<commit_message>
Code emitting for I/O operations implemented and tested.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -3885,8 +3885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J94" sqref="J94"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4653,7 +4653,7 @@
       <c r="D17" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="4" t="s">
         <v>216</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -4677,7 +4677,7 @@
       <c r="L17" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="4" t="s">
         <v>224</v>
       </c>
       <c r="N17" s="2" t="s">
@@ -4853,10 +4853,10 @@
       <c r="A24" s="1">
         <v>4</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>261</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -4871,16 +4871,16 @@
       <c r="G24" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="4" t="s">
         <v>266</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="4" t="s">
         <v>269</v>
       </c>
       <c r="L24" s="2" t="s">
@@ -4895,7 +4895,7 @@
       <c r="O24" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="P24" s="4" t="s">
         <v>273</v>
       </c>
       <c r="Q24" s="2" t="s">
@@ -4906,10 +4906,10 @@
       <c r="A25" s="1">
         <v>5</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="4" t="s">
         <v>276</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -4924,16 +4924,16 @@
       <c r="G25" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="4" t="s">
         <v>279</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K25" s="4" t="s">
         <v>282</v>
       </c>
       <c r="L25" s="2" t="s">
@@ -4948,7 +4948,7 @@
       <c r="O25" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="P25" s="2" t="s">
+      <c r="P25" s="4" t="s">
         <v>285</v>
       </c>
       <c r="Q25" s="2" t="s">
@@ -4959,10 +4959,10 @@
       <c r="A26" s="1">
         <v>6</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="4" t="s">
         <v>288</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -4977,16 +4977,16 @@
       <c r="G26" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="4" t="s">
         <v>266</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="4" t="s">
         <v>292</v>
       </c>
       <c r="L26" s="2" t="s">
@@ -5001,7 +5001,7 @@
       <c r="O26" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="P26" s="4" t="s">
         <v>273</v>
       </c>
       <c r="Q26" s="4" t="s">
@@ -5012,10 +5012,10 @@
       <c r="A27" s="1">
         <v>7</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="4" t="s">
         <v>296</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -5030,14 +5030,14 @@
       <c r="G27" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="4" t="s">
         <v>279</v>
       </c>
       <c r="I27" s="2"/>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="4" t="s">
         <v>300</v>
       </c>
       <c r="L27" s="2" t="s">
@@ -5052,7 +5052,7 @@
       <c r="O27" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="P27" s="2" t="s">
+      <c r="P27" s="4" t="s">
         <v>285</v>
       </c>
       <c r="Q27" s="2"/>

</xml_diff>

<commit_message>
Bit operations code emitting in progress
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -3886,7 +3886,7 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5403,52 +5403,52 @@
       <c r="A38" s="1">
         <v>4</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="I38" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="K38" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="L38" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="M38" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="N38" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="O38" s="2" t="s">
+      <c r="O38" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="P38" s="2" t="s">
+      <c r="P38" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="Q38" s="2" t="s">
+      <c r="Q38" s="4" t="s">
         <v>399</v>
       </c>
     </row>
@@ -5456,52 +5456,52 @@
       <c r="A39" s="1">
         <v>5</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="K39" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="L39" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="M39" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="N39" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="O39" s="2" t="s">
+      <c r="O39" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="P39" s="2" t="s">
+      <c r="P39" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="Q39" s="2" t="s">
+      <c r="Q39" s="4" t="s">
         <v>415</v>
       </c>
     </row>
@@ -5509,52 +5509,52 @@
       <c r="A40" s="1">
         <v>6</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="K40" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="L40" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="M40" s="2" t="s">
+      <c r="M40" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="N40" s="2" t="s">
+      <c r="N40" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="O40" s="2" t="s">
+      <c r="O40" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="P40" s="2" t="s">
+      <c r="P40" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="Q40" s="2" t="s">
+      <c r="Q40" s="4" t="s">
         <v>431</v>
       </c>
     </row>
@@ -5562,52 +5562,52 @@
       <c r="A41" s="1">
         <v>7</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I41" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="K41" s="2" t="s">
+      <c r="K41" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="L41" s="2" t="s">
+      <c r="L41" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="M41" s="2" t="s">
+      <c r="M41" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="N41" s="2" t="s">
+      <c r="N41" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="O41" s="2" t="s">
+      <c r="O41" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="P41" s="2" t="s">
+      <c r="P41" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="Q41" s="2" t="s">
+      <c r="Q41" s="4" t="s">
         <v>447</v>
       </c>
     </row>
@@ -5615,52 +5615,52 @@
       <c r="A42" s="1">
         <v>8</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="I42" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="J42" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="K42" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="L42" s="2" t="s">
+      <c r="L42" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="M42" s="2" t="s">
+      <c r="M42" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="N42" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="O42" s="2" t="s">
+      <c r="O42" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="P42" s="2" t="s">
+      <c r="P42" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="Q42" s="2" t="s">
+      <c r="Q42" s="4" t="s">
         <v>463</v>
       </c>
     </row>
@@ -5668,52 +5668,52 @@
       <c r="A43" s="1">
         <v>9</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H43" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="I43" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J43" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="K43" s="2" t="s">
+      <c r="K43" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="L43" s="2" t="s">
+      <c r="L43" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="M43" s="2" t="s">
+      <c r="M43" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="N43" s="2" t="s">
+      <c r="N43" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="O43" s="2" t="s">
+      <c r="O43" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="P43" s="2" t="s">
+      <c r="P43" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="Q43" s="2" t="s">
+      <c r="Q43" s="4" t="s">
         <v>479</v>
       </c>
     </row>
@@ -5721,52 +5721,52 @@
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="I44" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="J44" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="K44" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="L44" s="2" t="s">
+      <c r="L44" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="M44" s="2" t="s">
+      <c r="M44" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="N44" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="O44" s="2" t="s">
+      <c r="O44" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="P44" s="2" t="s">
+      <c r="P44" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="Q44" s="2" t="s">
+      <c r="Q44" s="4" t="s">
         <v>495</v>
       </c>
     </row>
@@ -5774,52 +5774,52 @@
       <c r="A45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H45" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="I45" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="J45" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="K45" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="L45" s="2" t="s">
+      <c r="L45" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="M45" s="2" t="s">
+      <c r="M45" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="N45" s="2" t="s">
+      <c r="N45" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="O45" s="2" t="s">
+      <c r="O45" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="P45" s="2" t="s">
+      <c r="P45" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="Q45" s="2" t="s">
+      <c r="Q45" s="4" t="s">
         <v>511</v>
       </c>
     </row>
@@ -5827,52 +5827,52 @@
       <c r="A46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="I46" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="J46" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="K46" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="L46" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="M46" s="2" t="s">
+      <c r="M46" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="N46" s="2" t="s">
+      <c r="N46" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="O46" s="2" t="s">
+      <c r="O46" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="P46" s="2" t="s">
+      <c r="P46" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="Q46" s="2" t="s">
+      <c r="Q46" s="4" t="s">
         <v>527</v>
       </c>
     </row>
@@ -5880,52 +5880,52 @@
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="I47" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="J47" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="K47" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="L47" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="M47" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="N47" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="O47" s="2" t="s">
+      <c r="O47" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="P47" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="Q47" s="2" t="s">
+      <c r="Q47" s="4" t="s">
         <v>543</v>
       </c>
     </row>
@@ -5933,52 +5933,52 @@
       <c r="A48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I48" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J48" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="K48" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="L48" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="M48" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="N48" s="2" t="s">
+      <c r="N48" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="O48" s="2" t="s">
+      <c r="O48" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="P48" s="2" t="s">
+      <c r="P48" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="Q48" s="2" t="s">
+      <c r="Q48" s="4" t="s">
         <v>559</v>
       </c>
     </row>
@@ -5986,52 +5986,52 @@
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G49" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="I49" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="J49" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="K49" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="L49" s="2" t="s">
+      <c r="L49" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="M49" s="2" t="s">
+      <c r="M49" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="N49" s="2" t="s">
+      <c r="N49" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="O49" s="2" t="s">
+      <c r="O49" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="P49" s="2" t="s">
+      <c r="P49" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="Q49" s="2" t="s">
+      <c r="Q49" s="4" t="s">
         <v>575</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code emitting for bit test and manipulation operators implemented and tested.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -3885,8 +3885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6869,52 +6869,52 @@
       <c r="A78" s="1">
         <v>4</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="J78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="K78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="L78" s="2" t="s">
+      <c r="L78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="M78" s="2" t="s">
+      <c r="M78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="N78" s="2" t="s">
+      <c r="N78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="O78" s="2" t="s">
+      <c r="O78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="P78" s="2" t="s">
+      <c r="P78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="Q78" s="2" t="s">
+      <c r="Q78" s="4" t="s">
         <v>728</v>
       </c>
     </row>
@@ -6922,52 +6922,52 @@
       <c r="A79" s="1">
         <v>5</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="H79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="J79" s="2" t="s">
+      <c r="J79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="K79" s="2" t="s">
+      <c r="K79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="L79" s="2" t="s">
+      <c r="L79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="M79" s="2" t="s">
+      <c r="M79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="N79" s="2" t="s">
+      <c r="N79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="O79" s="2" t="s">
+      <c r="O79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="P79" s="2" t="s">
+      <c r="P79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="Q79" s="2" t="s">
+      <c r="Q79" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -6975,52 +6975,52 @@
       <c r="A80" s="1">
         <v>6</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="G80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="H80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="I80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="J80" s="2" t="s">
+      <c r="J80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="K80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="L80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="M80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="N80" s="2" t="s">
+      <c r="N80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="O80" s="2" t="s">
+      <c r="O80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="P80" s="2" t="s">
+      <c r="P80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="Q80" s="2" t="s">
+      <c r="Q80" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -7028,52 +7028,52 @@
       <c r="A81" s="1">
         <v>7</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="G81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="H81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="I81" s="2" t="s">
+      <c r="I81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="J81" s="2" t="s">
+      <c r="J81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="K81" s="2" t="s">
+      <c r="K81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="L81" s="2" t="s">
+      <c r="L81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="M81" s="2" t="s">
+      <c r="M81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="N81" s="2" t="s">
+      <c r="N81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="O81" s="2" t="s">
+      <c r="O81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="P81" s="2" t="s">
+      <c r="P81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="Q81" s="2" t="s">
+      <c r="Q81" s="4" t="s">
         <v>734</v>
       </c>
     </row>
@@ -7081,52 +7081,52 @@
       <c r="A82" s="1">
         <v>8</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D82" s="4" t="s">
         <v>737</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="E82" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F82" s="4" t="s">
         <v>739</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="G82" s="4" t="s">
         <v>740</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H82" s="4" t="s">
         <v>741</v>
       </c>
-      <c r="I82" s="2" t="s">
+      <c r="I82" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="J82" s="4" t="s">
         <v>743</v>
       </c>
-      <c r="K82" s="2" t="s">
+      <c r="K82" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="L82" s="2" t="s">
+      <c r="L82" s="4" t="s">
         <v>745</v>
       </c>
-      <c r="M82" s="2" t="s">
+      <c r="M82" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="N82" s="2" t="s">
+      <c r="N82" s="4" t="s">
         <v>747</v>
       </c>
-      <c r="O82" s="2" t="s">
+      <c r="O82" s="4" t="s">
         <v>748</v>
       </c>
-      <c r="P82" s="2" t="s">
+      <c r="P82" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="Q82" s="2" t="s">
+      <c r="Q82" s="4" t="s">
         <v>750</v>
       </c>
     </row>
@@ -7134,52 +7134,52 @@
       <c r="A83" s="1">
         <v>9</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="4" t="s">
         <v>751</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="4" t="s">
         <v>752</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D83" s="4" t="s">
         <v>753</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="E83" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F83" s="4" t="s">
         <v>755</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G83" s="4" t="s">
         <v>756</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="H83" s="4" t="s">
         <v>757</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="I83" s="4" t="s">
         <v>758</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="J83" s="4" t="s">
         <v>759</v>
       </c>
-      <c r="K83" s="2" t="s">
+      <c r="K83" s="4" t="s">
         <v>760</v>
       </c>
-      <c r="L83" s="2" t="s">
+      <c r="L83" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="M83" s="2" t="s">
+      <c r="M83" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="N83" s="2" t="s">
+      <c r="N83" s="4" t="s">
         <v>763</v>
       </c>
-      <c r="O83" s="2" t="s">
+      <c r="O83" s="4" t="s">
         <v>764</v>
       </c>
-      <c r="P83" s="2" t="s">
+      <c r="P83" s="4" t="s">
         <v>765</v>
       </c>
-      <c r="Q83" s="2" t="s">
+      <c r="Q83" s="4" t="s">
         <v>766</v>
       </c>
     </row>
@@ -7187,52 +7187,52 @@
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="4" t="s">
         <v>767</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="4" t="s">
         <v>768</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D84" s="4" t="s">
         <v>769</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="E84" s="4" t="s">
         <v>770</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F84" s="4" t="s">
         <v>771</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="G84" s="4" t="s">
         <v>772</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="H84" s="4" t="s">
         <v>773</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I84" s="4" t="s">
         <v>774</v>
       </c>
-      <c r="J84" s="2" t="s">
+      <c r="J84" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="K84" s="2" t="s">
+      <c r="K84" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="L84" s="2" t="s">
+      <c r="L84" s="4" t="s">
         <v>777</v>
       </c>
-      <c r="M84" s="2" t="s">
+      <c r="M84" s="4" t="s">
         <v>778</v>
       </c>
-      <c r="N84" s="2" t="s">
+      <c r="N84" s="4" t="s">
         <v>779</v>
       </c>
-      <c r="O84" s="2" t="s">
+      <c r="O84" s="4" t="s">
         <v>780</v>
       </c>
-      <c r="P84" s="2" t="s">
+      <c r="P84" s="4" t="s">
         <v>781</v>
       </c>
-      <c r="Q84" s="2" t="s">
+      <c r="Q84" s="4" t="s">
         <v>782</v>
       </c>
     </row>
@@ -7240,52 +7240,52 @@
       <c r="A85" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="4" t="s">
         <v>783</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="4" t="s">
         <v>784</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D85" s="4" t="s">
         <v>785</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E85" s="4" t="s">
         <v>786</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F85" s="4" t="s">
         <v>787</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="G85" s="4" t="s">
         <v>788</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="H85" s="4" t="s">
         <v>789</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="I85" s="4" t="s">
         <v>790</v>
       </c>
-      <c r="J85" s="2" t="s">
+      <c r="J85" s="4" t="s">
         <v>791</v>
       </c>
-      <c r="K85" s="2" t="s">
+      <c r="K85" s="4" t="s">
         <v>792</v>
       </c>
-      <c r="L85" s="2" t="s">
+      <c r="L85" s="4" t="s">
         <v>793</v>
       </c>
-      <c r="M85" s="2" t="s">
+      <c r="M85" s="4" t="s">
         <v>794</v>
       </c>
-      <c r="N85" s="2" t="s">
+      <c r="N85" s="4" t="s">
         <v>795</v>
       </c>
-      <c r="O85" s="2" t="s">
+      <c r="O85" s="4" t="s">
         <v>796</v>
       </c>
-      <c r="P85" s="2" t="s">
+      <c r="P85" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="Q85" s="2" t="s">
+      <c r="Q85" s="4" t="s">
         <v>798</v>
       </c>
     </row>
@@ -7293,52 +7293,52 @@
       <c r="A86" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="4" t="s">
         <v>799</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="4" t="s">
         <v>800</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D86" s="4" t="s">
         <v>801</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E86" s="4" t="s">
         <v>802</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F86" s="4" t="s">
         <v>803</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="G86" s="4" t="s">
         <v>804</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="H86" s="4" t="s">
         <v>805</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="I86" s="4" t="s">
         <v>806</v>
       </c>
-      <c r="J86" s="2" t="s">
+      <c r="J86" s="4" t="s">
         <v>807</v>
       </c>
-      <c r="K86" s="2" t="s">
+      <c r="K86" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="L86" s="2" t="s">
+      <c r="L86" s="4" t="s">
         <v>809</v>
       </c>
-      <c r="M86" s="2" t="s">
+      <c r="M86" s="4" t="s">
         <v>810</v>
       </c>
-      <c r="N86" s="2" t="s">
+      <c r="N86" s="4" t="s">
         <v>811</v>
       </c>
-      <c r="O86" s="2" t="s">
+      <c r="O86" s="4" t="s">
         <v>812</v>
       </c>
-      <c r="P86" s="2" t="s">
+      <c r="P86" s="4" t="s">
         <v>813</v>
       </c>
-      <c r="Q86" s="2" t="s">
+      <c r="Q86" s="4" t="s">
         <v>814</v>
       </c>
     </row>
@@ -7346,52 +7346,52 @@
       <c r="A87" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="4" t="s">
         <v>815</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="4" t="s">
         <v>816</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="D87" s="4" t="s">
         <v>817</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="E87" s="4" t="s">
         <v>818</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F87" s="4" t="s">
         <v>819</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G87" s="4" t="s">
         <v>820</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="H87" s="4" t="s">
         <v>821</v>
       </c>
-      <c r="I87" s="2" t="s">
+      <c r="I87" s="4" t="s">
         <v>822</v>
       </c>
-      <c r="J87" s="2" t="s">
+      <c r="J87" s="4" t="s">
         <v>823</v>
       </c>
-      <c r="K87" s="2" t="s">
+      <c r="K87" s="4" t="s">
         <v>824</v>
       </c>
-      <c r="L87" s="2" t="s">
+      <c r="L87" s="4" t="s">
         <v>825</v>
       </c>
-      <c r="M87" s="2" t="s">
+      <c r="M87" s="4" t="s">
         <v>826</v>
       </c>
-      <c r="N87" s="2" t="s">
+      <c r="N87" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="O87" s="2" t="s">
+      <c r="O87" s="4" t="s">
         <v>828</v>
       </c>
-      <c r="P87" s="2" t="s">
+      <c r="P87" s="4" t="s">
         <v>829</v>
       </c>
-      <c r="Q87" s="2" t="s">
+      <c r="Q87" s="4" t="s">
         <v>830</v>
       </c>
     </row>
@@ -7399,52 +7399,52 @@
       <c r="A88" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="4" t="s">
         <v>831</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="4" t="s">
         <v>832</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D88" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E88" s="4" t="s">
         <v>834</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F88" s="4" t="s">
         <v>835</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G88" s="4" t="s">
         <v>836</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="H88" s="4" t="s">
         <v>837</v>
       </c>
-      <c r="I88" s="2" t="s">
+      <c r="I88" s="4" t="s">
         <v>838</v>
       </c>
-      <c r="J88" s="2" t="s">
+      <c r="J88" s="4" t="s">
         <v>839</v>
       </c>
-      <c r="K88" s="2" t="s">
+      <c r="K88" s="4" t="s">
         <v>840</v>
       </c>
-      <c r="L88" s="2" t="s">
+      <c r="L88" s="4" t="s">
         <v>841</v>
       </c>
-      <c r="M88" s="2" t="s">
+      <c r="M88" s="4" t="s">
         <v>842</v>
       </c>
-      <c r="N88" s="2" t="s">
+      <c r="N88" s="4" t="s">
         <v>843</v>
       </c>
-      <c r="O88" s="2" t="s">
+      <c r="O88" s="4" t="s">
         <v>844</v>
       </c>
-      <c r="P88" s="2" t="s">
+      <c r="P88" s="4" t="s">
         <v>845</v>
       </c>
-      <c r="Q88" s="2" t="s">
+      <c r="Q88" s="4" t="s">
         <v>846</v>
       </c>
     </row>
@@ -7452,52 +7452,52 @@
       <c r="A89" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="4" t="s">
         <v>847</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="4" t="s">
         <v>848</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D89" s="4" t="s">
         <v>849</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E89" s="4" t="s">
         <v>850</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F89" s="4" t="s">
         <v>851</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="G89" s="4" t="s">
         <v>852</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="H89" s="4" t="s">
         <v>853</v>
       </c>
-      <c r="I89" s="2" t="s">
+      <c r="I89" s="4" t="s">
         <v>854</v>
       </c>
-      <c r="J89" s="2" t="s">
+      <c r="J89" s="4" t="s">
         <v>855</v>
       </c>
-      <c r="K89" s="2" t="s">
+      <c r="K89" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="L89" s="2" t="s">
+      <c r="L89" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="M89" s="2" t="s">
+      <c r="M89" s="4" t="s">
         <v>858</v>
       </c>
-      <c r="N89" s="2" t="s">
+      <c r="N89" s="4" t="s">
         <v>859</v>
       </c>
-      <c r="O89" s="2" t="s">
+      <c r="O89" s="4" t="s">
         <v>860</v>
       </c>
-      <c r="P89" s="2" t="s">
+      <c r="P89" s="4" t="s">
         <v>861</v>
       </c>
-      <c r="Q89" s="2" t="s">
+      <c r="Q89" s="4" t="s">
         <v>862</v>
       </c>
     </row>
@@ -8335,52 +8335,52 @@
       <c r="A118" s="1">
         <v>4</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="D118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="E118" s="2" t="s">
+      <c r="E118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="F118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="G118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="H118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="I118" s="2" t="s">
+      <c r="I118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="J118" s="2" t="s">
+      <c r="J118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="K118" s="2" t="s">
+      <c r="K118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="L118" s="2" t="s">
+      <c r="L118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="M118" s="2" t="s">
+      <c r="M118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="N118" s="2" t="s">
+      <c r="N118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="O118" s="2" t="s">
+      <c r="O118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="P118" s="2" t="s">
+      <c r="P118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="Q118" s="2" t="s">
+      <c r="Q118" s="4" t="s">
         <v>1015</v>
       </c>
     </row>
@@ -8388,52 +8388,52 @@
       <c r="A119" s="1">
         <v>5</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="D119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="E119" s="2" t="s">
+      <c r="E119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="F119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="G119" s="2" t="s">
+      <c r="G119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="H119" s="2" t="s">
+      <c r="H119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="I119" s="2" t="s">
+      <c r="I119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="J119" s="2" t="s">
+      <c r="J119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="K119" s="2" t="s">
+      <c r="K119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="L119" s="2" t="s">
+      <c r="L119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="M119" s="2" t="s">
+      <c r="M119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="N119" s="2" t="s">
+      <c r="N119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="O119" s="2" t="s">
+      <c r="O119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="P119" s="2" t="s">
+      <c r="P119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="Q119" s="2" t="s">
+      <c r="Q119" s="4" t="s">
         <v>1017</v>
       </c>
     </row>
@@ -8441,52 +8441,52 @@
       <c r="A120" s="1">
         <v>6</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="D120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="E120" s="2" t="s">
+      <c r="E120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="F120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="G120" s="2" t="s">
+      <c r="G120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="H120" s="2" t="s">
+      <c r="H120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="I120" s="2" t="s">
+      <c r="I120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="J120" s="2" t="s">
+      <c r="J120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="K120" s="2" t="s">
+      <c r="K120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="L120" s="2" t="s">
+      <c r="L120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="M120" s="2" t="s">
+      <c r="M120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="N120" s="2" t="s">
+      <c r="N120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="O120" s="2" t="s">
+      <c r="O120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="P120" s="2" t="s">
+      <c r="P120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="Q120" s="2" t="s">
+      <c r="Q120" s="4" t="s">
         <v>1019</v>
       </c>
     </row>
@@ -8494,52 +8494,52 @@
       <c r="A121" s="1">
         <v>7</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="E121" s="2" t="s">
+      <c r="E121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="F121" s="2" t="s">
+      <c r="F121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="G121" s="2" t="s">
+      <c r="G121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="H121" s="2" t="s">
+      <c r="H121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="I121" s="2" t="s">
+      <c r="I121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="J121" s="2" t="s">
+      <c r="J121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="K121" s="2" t="s">
+      <c r="K121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="L121" s="2" t="s">
+      <c r="L121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="M121" s="2" t="s">
+      <c r="M121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="N121" s="2" t="s">
+      <c r="N121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="O121" s="2" t="s">
+      <c r="O121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="P121" s="2" t="s">
+      <c r="P121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="Q121" s="2" t="s">
+      <c r="Q121" s="4" t="s">
         <v>1021</v>
       </c>
     </row>
@@ -8547,52 +8547,52 @@
       <c r="A122" s="1">
         <v>8</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="4" t="s">
         <v>1022</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="4" t="s">
         <v>1023</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D122" s="4" t="s">
         <v>1024</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="E122" s="4" t="s">
         <v>1025</v>
       </c>
-      <c r="F122" s="2" t="s">
+      <c r="F122" s="4" t="s">
         <v>1026</v>
       </c>
-      <c r="G122" s="2" t="s">
+      <c r="G122" s="4" t="s">
         <v>1027</v>
       </c>
-      <c r="H122" s="2" t="s">
+      <c r="H122" s="4" t="s">
         <v>1028</v>
       </c>
-      <c r="I122" s="2" t="s">
+      <c r="I122" s="4" t="s">
         <v>1029</v>
       </c>
-      <c r="J122" s="2" t="s">
+      <c r="J122" s="4" t="s">
         <v>1030</v>
       </c>
-      <c r="K122" s="2" t="s">
+      <c r="K122" s="4" t="s">
         <v>1031</v>
       </c>
-      <c r="L122" s="2" t="s">
+      <c r="L122" s="4" t="s">
         <v>1032</v>
       </c>
-      <c r="M122" s="2" t="s">
+      <c r="M122" s="4" t="s">
         <v>1033</v>
       </c>
-      <c r="N122" s="2" t="s">
+      <c r="N122" s="4" t="s">
         <v>1034</v>
       </c>
-      <c r="O122" s="2" t="s">
+      <c r="O122" s="4" t="s">
         <v>1035</v>
       </c>
-      <c r="P122" s="2" t="s">
+      <c r="P122" s="4" t="s">
         <v>1036</v>
       </c>
-      <c r="Q122" s="2" t="s">
+      <c r="Q122" s="4" t="s">
         <v>1037</v>
       </c>
     </row>
@@ -8600,52 +8600,52 @@
       <c r="A123" s="1">
         <v>9</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="4" t="s">
         <v>1038</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="4" t="s">
         <v>1039</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D123" s="4" t="s">
         <v>1040</v>
       </c>
-      <c r="E123" s="2" t="s">
+      <c r="E123" s="4" t="s">
         <v>1041</v>
       </c>
-      <c r="F123" s="2" t="s">
+      <c r="F123" s="4" t="s">
         <v>1042</v>
       </c>
-      <c r="G123" s="2" t="s">
+      <c r="G123" s="4" t="s">
         <v>1043</v>
       </c>
-      <c r="H123" s="2" t="s">
+      <c r="H123" s="4" t="s">
         <v>1044</v>
       </c>
-      <c r="I123" s="2" t="s">
+      <c r="I123" s="4" t="s">
         <v>1045</v>
       </c>
-      <c r="J123" s="2" t="s">
+      <c r="J123" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="K123" s="2" t="s">
+      <c r="K123" s="4" t="s">
         <v>1047</v>
       </c>
-      <c r="L123" s="2" t="s">
+      <c r="L123" s="4" t="s">
         <v>1048</v>
       </c>
-      <c r="M123" s="2" t="s">
+      <c r="M123" s="4" t="s">
         <v>1049</v>
       </c>
-      <c r="N123" s="2" t="s">
+      <c r="N123" s="4" t="s">
         <v>1050</v>
       </c>
-      <c r="O123" s="2" t="s">
+      <c r="O123" s="4" t="s">
         <v>1051</v>
       </c>
-      <c r="P123" s="2" t="s">
+      <c r="P123" s="4" t="s">
         <v>1052</v>
       </c>
-      <c r="Q123" s="2" t="s">
+      <c r="Q123" s="4" t="s">
         <v>1053</v>
       </c>
     </row>
@@ -8653,52 +8653,52 @@
       <c r="A124" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" s="4" t="s">
         <v>1054</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="4" t="s">
         <v>1055</v>
       </c>
-      <c r="D124" s="2" t="s">
+      <c r="D124" s="4" t="s">
         <v>1056</v>
       </c>
-      <c r="E124" s="2" t="s">
+      <c r="E124" s="4" t="s">
         <v>1057</v>
       </c>
-      <c r="F124" s="2" t="s">
+      <c r="F124" s="4" t="s">
         <v>1058</v>
       </c>
-      <c r="G124" s="2" t="s">
+      <c r="G124" s="4" t="s">
         <v>1059</v>
       </c>
-      <c r="H124" s="2" t="s">
+      <c r="H124" s="4" t="s">
         <v>1060</v>
       </c>
-      <c r="I124" s="2" t="s">
+      <c r="I124" s="4" t="s">
         <v>1061</v>
       </c>
-      <c r="J124" s="2" t="s">
+      <c r="J124" s="4" t="s">
         <v>1062</v>
       </c>
-      <c r="K124" s="2" t="s">
+      <c r="K124" s="4" t="s">
         <v>1063</v>
       </c>
-      <c r="L124" s="2" t="s">
+      <c r="L124" s="4" t="s">
         <v>1064</v>
       </c>
-      <c r="M124" s="2" t="s">
+      <c r="M124" s="4" t="s">
         <v>1065</v>
       </c>
-      <c r="N124" s="2" t="s">
+      <c r="N124" s="4" t="s">
         <v>1066</v>
       </c>
-      <c r="O124" s="2" t="s">
+      <c r="O124" s="4" t="s">
         <v>1067</v>
       </c>
-      <c r="P124" s="2" t="s">
+      <c r="P124" s="4" t="s">
         <v>1068</v>
       </c>
-      <c r="Q124" s="2" t="s">
+      <c r="Q124" s="4" t="s">
         <v>1069</v>
       </c>
     </row>
@@ -8706,52 +8706,52 @@
       <c r="A125" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B125" s="4" t="s">
         <v>1070</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="4" t="s">
         <v>1071</v>
       </c>
-      <c r="D125" s="2" t="s">
+      <c r="D125" s="4" t="s">
         <v>1072</v>
       </c>
-      <c r="E125" s="2" t="s">
+      <c r="E125" s="4" t="s">
         <v>1073</v>
       </c>
-      <c r="F125" s="2" t="s">
+      <c r="F125" s="4" t="s">
         <v>1074</v>
       </c>
-      <c r="G125" s="2" t="s">
+      <c r="G125" s="4" t="s">
         <v>1075</v>
       </c>
-      <c r="H125" s="2" t="s">
+      <c r="H125" s="4" t="s">
         <v>1076</v>
       </c>
-      <c r="I125" s="2" t="s">
+      <c r="I125" s="4" t="s">
         <v>1077</v>
       </c>
-      <c r="J125" s="2" t="s">
+      <c r="J125" s="4" t="s">
         <v>1078</v>
       </c>
-      <c r="K125" s="2" t="s">
+      <c r="K125" s="4" t="s">
         <v>1079</v>
       </c>
-      <c r="L125" s="2" t="s">
+      <c r="L125" s="4" t="s">
         <v>1080</v>
       </c>
-      <c r="M125" s="2" t="s">
+      <c r="M125" s="4" t="s">
         <v>1081</v>
       </c>
-      <c r="N125" s="2" t="s">
+      <c r="N125" s="4" t="s">
         <v>1082</v>
       </c>
-      <c r="O125" s="2" t="s">
+      <c r="O125" s="4" t="s">
         <v>1083</v>
       </c>
-      <c r="P125" s="2" t="s">
+      <c r="P125" s="4" t="s">
         <v>1084</v>
       </c>
-      <c r="Q125" s="2" t="s">
+      <c r="Q125" s="4" t="s">
         <v>1085</v>
       </c>
     </row>
@@ -8759,52 +8759,52 @@
       <c r="A126" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B126" s="4" t="s">
         <v>1086</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="4" t="s">
         <v>1087</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="D126" s="4" t="s">
         <v>1088</v>
       </c>
-      <c r="E126" s="2" t="s">
+      <c r="E126" s="4" t="s">
         <v>1089</v>
       </c>
-      <c r="F126" s="2" t="s">
+      <c r="F126" s="4" t="s">
         <v>1090</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="G126" s="4" t="s">
         <v>1091</v>
       </c>
-      <c r="H126" s="2" t="s">
+      <c r="H126" s="4" t="s">
         <v>1092</v>
       </c>
-      <c r="I126" s="2" t="s">
+      <c r="I126" s="4" t="s">
         <v>1093</v>
       </c>
-      <c r="J126" s="2" t="s">
+      <c r="J126" s="4" t="s">
         <v>1094</v>
       </c>
-      <c r="K126" s="2" t="s">
+      <c r="K126" s="4" t="s">
         <v>1095</v>
       </c>
-      <c r="L126" s="2" t="s">
+      <c r="L126" s="4" t="s">
         <v>1096</v>
       </c>
-      <c r="M126" s="2" t="s">
+      <c r="M126" s="4" t="s">
         <v>1097</v>
       </c>
-      <c r="N126" s="2" t="s">
+      <c r="N126" s="4" t="s">
         <v>1098</v>
       </c>
-      <c r="O126" s="2" t="s">
+      <c r="O126" s="4" t="s">
         <v>1099</v>
       </c>
-      <c r="P126" s="2" t="s">
+      <c r="P126" s="4" t="s">
         <v>1100</v>
       </c>
-      <c r="Q126" s="2" t="s">
+      <c r="Q126" s="4" t="s">
         <v>1101</v>
       </c>
     </row>
@@ -8812,52 +8812,52 @@
       <c r="A127" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="4" t="s">
         <v>1102</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="4" t="s">
         <v>1103</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D127" s="4" t="s">
         <v>1104</v>
       </c>
-      <c r="E127" s="2" t="s">
+      <c r="E127" s="4" t="s">
         <v>1105</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="F127" s="4" t="s">
         <v>1106</v>
       </c>
-      <c r="G127" s="2" t="s">
+      <c r="G127" s="4" t="s">
         <v>1107</v>
       </c>
-      <c r="H127" s="2" t="s">
+      <c r="H127" s="4" t="s">
         <v>1108</v>
       </c>
-      <c r="I127" s="2" t="s">
+      <c r="I127" s="4" t="s">
         <v>1109</v>
       </c>
-      <c r="J127" s="2" t="s">
+      <c r="J127" s="4" t="s">
         <v>1110</v>
       </c>
-      <c r="K127" s="2" t="s">
+      <c r="K127" s="4" t="s">
         <v>1111</v>
       </c>
-      <c r="L127" s="2" t="s">
+      <c r="L127" s="4" t="s">
         <v>1112</v>
       </c>
-      <c r="M127" s="2" t="s">
+      <c r="M127" s="4" t="s">
         <v>1113</v>
       </c>
-      <c r="N127" s="2" t="s">
+      <c r="N127" s="4" t="s">
         <v>1114</v>
       </c>
-      <c r="O127" s="2" t="s">
+      <c r="O127" s="4" t="s">
         <v>1115</v>
       </c>
-      <c r="P127" s="2" t="s">
+      <c r="P127" s="4" t="s">
         <v>1116</v>
       </c>
-      <c r="Q127" s="2" t="s">
+      <c r="Q127" s="4" t="s">
         <v>1117</v>
       </c>
     </row>
@@ -8865,52 +8865,52 @@
       <c r="A128" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="4" t="s">
         <v>1118</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="4" t="s">
         <v>1119</v>
       </c>
-      <c r="D128" s="2" t="s">
+      <c r="D128" s="4" t="s">
         <v>1120</v>
       </c>
-      <c r="E128" s="2" t="s">
+      <c r="E128" s="4" t="s">
         <v>1121</v>
       </c>
-      <c r="F128" s="2" t="s">
+      <c r="F128" s="4" t="s">
         <v>1122</v>
       </c>
-      <c r="G128" s="2" t="s">
+      <c r="G128" s="4" t="s">
         <v>1123</v>
       </c>
-      <c r="H128" s="2" t="s">
+      <c r="H128" s="4" t="s">
         <v>1124</v>
       </c>
-      <c r="I128" s="2" t="s">
+      <c r="I128" s="4" t="s">
         <v>1125</v>
       </c>
-      <c r="J128" s="2" t="s">
+      <c r="J128" s="4" t="s">
         <v>1126</v>
       </c>
-      <c r="K128" s="2" t="s">
+      <c r="K128" s="4" t="s">
         <v>1127</v>
       </c>
-      <c r="L128" s="2" t="s">
+      <c r="L128" s="4" t="s">
         <v>1128</v>
       </c>
-      <c r="M128" s="2" t="s">
+      <c r="M128" s="4" t="s">
         <v>1129</v>
       </c>
-      <c r="N128" s="2" t="s">
+      <c r="N128" s="4" t="s">
         <v>1130</v>
       </c>
-      <c r="O128" s="2" t="s">
+      <c r="O128" s="4" t="s">
         <v>1131</v>
       </c>
-      <c r="P128" s="2" t="s">
+      <c r="P128" s="4" t="s">
         <v>1132</v>
       </c>
-      <c r="Q128" s="2" t="s">
+      <c r="Q128" s="4" t="s">
         <v>1133</v>
       </c>
     </row>
@@ -8918,52 +8918,52 @@
       <c r="A129" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" s="4" t="s">
         <v>1134</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="4" t="s">
         <v>1135</v>
       </c>
-      <c r="D129" s="2" t="s">
+      <c r="D129" s="4" t="s">
         <v>1136</v>
       </c>
-      <c r="E129" s="2" t="s">
+      <c r="E129" s="4" t="s">
         <v>1137</v>
       </c>
-      <c r="F129" s="2" t="s">
+      <c r="F129" s="4" t="s">
         <v>1138</v>
       </c>
-      <c r="G129" s="2" t="s">
+      <c r="G129" s="4" t="s">
         <v>1139</v>
       </c>
-      <c r="H129" s="2" t="s">
+      <c r="H129" s="4" t="s">
         <v>1140</v>
       </c>
-      <c r="I129" s="2" t="s">
+      <c r="I129" s="4" t="s">
         <v>1141</v>
       </c>
-      <c r="J129" s="2" t="s">
+      <c r="J129" s="4" t="s">
         <v>1142</v>
       </c>
-      <c r="K129" s="2" t="s">
+      <c r="K129" s="4" t="s">
         <v>1143</v>
       </c>
-      <c r="L129" s="2" t="s">
+      <c r="L129" s="4" t="s">
         <v>1144</v>
       </c>
-      <c r="M129" s="2" t="s">
+      <c r="M129" s="4" t="s">
         <v>1145</v>
       </c>
-      <c r="N129" s="2" t="s">
+      <c r="N129" s="4" t="s">
         <v>1146</v>
       </c>
-      <c r="O129" s="2" t="s">
+      <c r="O129" s="4" t="s">
         <v>1147</v>
       </c>
-      <c r="P129" s="2" t="s">
+      <c r="P129" s="4" t="s">
         <v>1148</v>
       </c>
-      <c r="Q129" s="2" t="s">
+      <c r="Q129" s="4" t="s">
         <v>1149</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code emitting for shift and rotate operations implemented and tested.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -3885,8 +3885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5191,52 +5191,52 @@
       <c r="A34" s="1">
         <v>0</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="K34" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="L34" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="M34" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="N34" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="O34" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="P34" s="2" t="s">
+      <c r="P34" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="Q34" s="2" t="s">
+      <c r="Q34" s="4" t="s">
         <v>335</v>
       </c>
     </row>
@@ -5244,52 +5244,52 @@
       <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="I35" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="K35" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="L35" s="2" t="s">
+      <c r="L35" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="M35" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="N35" s="2" t="s">
+      <c r="N35" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="O35" s="2" t="s">
+      <c r="O35" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="P35" s="2" t="s">
+      <c r="P35" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="Q35" s="2" t="s">
+      <c r="Q35" s="4" t="s">
         <v>351</v>
       </c>
     </row>
@@ -5297,52 +5297,52 @@
       <c r="A36" s="1">
         <v>2</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="I36" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="K36" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="L36" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="M36" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="N36" s="2" t="s">
+      <c r="N36" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="O36" s="2" t="s">
+      <c r="O36" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="P36" s="2" t="s">
+      <c r="P36" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="Q36" s="2" t="s">
+      <c r="Q36" s="4" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5350,52 +5350,52 @@
       <c r="A37" s="1">
         <v>3</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="I37" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="K37" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="L37" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="M37" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="N37" s="2" t="s">
+      <c r="N37" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="O37" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="P37" s="2" t="s">
+      <c r="P37" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="Q37" s="2" t="s">
+      <c r="Q37" s="4" t="s">
         <v>383</v>
       </c>
     </row>
@@ -6657,52 +6657,52 @@
       <c r="A74" s="1">
         <v>0</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E74" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="H74" s="4" t="s">
         <v>669</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="I74" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="J74" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="K74" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="L74" s="2" t="s">
+      <c r="L74" s="4" t="s">
         <v>673</v>
       </c>
-      <c r="M74" s="2" t="s">
+      <c r="M74" s="4" t="s">
         <v>674</v>
       </c>
-      <c r="N74" s="2" t="s">
+      <c r="N74" s="4" t="s">
         <v>675</v>
       </c>
-      <c r="O74" s="2" t="s">
+      <c r="O74" s="4" t="s">
         <v>676</v>
       </c>
-      <c r="P74" s="2" t="s">
+      <c r="P74" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="Q74" s="2" t="s">
+      <c r="Q74" s="4" t="s">
         <v>678</v>
       </c>
     </row>
@@ -6710,52 +6710,52 @@
       <c r="A75" s="1">
         <v>1</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="4" t="s">
         <v>680</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" s="4" t="s">
         <v>681</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F75" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" s="4" t="s">
         <v>684</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H75" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="I75" s="4" t="s">
         <v>686</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="J75" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="K75" s="4" t="s">
         <v>688</v>
       </c>
-      <c r="L75" s="2" t="s">
+      <c r="L75" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="M75" s="2" t="s">
+      <c r="M75" s="4" t="s">
         <v>690</v>
       </c>
-      <c r="N75" s="2" t="s">
+      <c r="N75" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="O75" s="2" t="s">
+      <c r="O75" s="4" t="s">
         <v>692</v>
       </c>
-      <c r="P75" s="2" t="s">
+      <c r="P75" s="4" t="s">
         <v>693</v>
       </c>
-      <c r="Q75" s="2" t="s">
+      <c r="Q75" s="4" t="s">
         <v>694</v>
       </c>
     </row>
@@ -6763,52 +6763,52 @@
       <c r="A76" s="1">
         <v>2</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E76" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F76" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G76" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="H76" s="4" t="s">
         <v>701</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="I76" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="J76" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="K76" s="2" t="s">
+      <c r="K76" s="4" t="s">
         <v>704</v>
       </c>
-      <c r="L76" s="2" t="s">
+      <c r="L76" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="M76" s="2" t="s">
+      <c r="M76" s="4" t="s">
         <v>706</v>
       </c>
-      <c r="N76" s="2" t="s">
+      <c r="N76" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="O76" s="2" t="s">
+      <c r="O76" s="4" t="s">
         <v>708</v>
       </c>
-      <c r="P76" s="2" t="s">
+      <c r="P76" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="Q76" s="2" t="s">
+      <c r="Q76" s="4" t="s">
         <v>710</v>
       </c>
     </row>
@@ -6816,52 +6816,52 @@
       <c r="A77" s="1">
         <v>3</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D77" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E77" s="4" t="s">
         <v>714</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F77" s="4" t="s">
         <v>715</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G77" s="4" t="s">
         <v>716</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="H77" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="I77" s="4" t="s">
         <v>718</v>
       </c>
-      <c r="J77" s="2" t="s">
+      <c r="J77" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="K77" s="2" t="s">
+      <c r="K77" s="4" t="s">
         <v>720</v>
       </c>
-      <c r="L77" s="2" t="s">
+      <c r="L77" s="4" t="s">
         <v>721</v>
       </c>
-      <c r="M77" s="2" t="s">
+      <c r="M77" s="4" t="s">
         <v>722</v>
       </c>
-      <c r="N77" s="2" t="s">
+      <c r="N77" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="O77" s="2" t="s">
+      <c r="O77" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="P77" s="2" t="s">
+      <c r="P77" s="4" t="s">
         <v>725</v>
       </c>
-      <c r="Q77" s="2" t="s">
+      <c r="Q77" s="4" t="s">
         <v>726</v>
       </c>
     </row>
@@ -8123,52 +8123,52 @@
       <c r="A114" s="1">
         <v>0</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="4" t="s">
         <v>950</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="4" t="s">
         <v>951</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D114" s="4" t="s">
         <v>952</v>
       </c>
-      <c r="E114" s="2" t="s">
+      <c r="E114" s="4" t="s">
         <v>953</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="F114" s="4" t="s">
         <v>954</v>
       </c>
-      <c r="G114" s="2" t="s">
+      <c r="G114" s="4" t="s">
         <v>955</v>
       </c>
-      <c r="H114" s="2" t="s">
+      <c r="H114" s="4" t="s">
         <v>956</v>
       </c>
-      <c r="I114" s="2" t="s">
+      <c r="I114" s="4" t="s">
         <v>957</v>
       </c>
-      <c r="J114" s="2" t="s">
+      <c r="J114" s="4" t="s">
         <v>958</v>
       </c>
-      <c r="K114" s="2" t="s">
+      <c r="K114" s="4" t="s">
         <v>959</v>
       </c>
-      <c r="L114" s="2" t="s">
+      <c r="L114" s="4" t="s">
         <v>960</v>
       </c>
-      <c r="M114" s="2" t="s">
+      <c r="M114" s="4" t="s">
         <v>961</v>
       </c>
-      <c r="N114" s="2" t="s">
+      <c r="N114" s="4" t="s">
         <v>962</v>
       </c>
-      <c r="O114" s="2" t="s">
+      <c r="O114" s="4" t="s">
         <v>963</v>
       </c>
-      <c r="P114" s="2" t="s">
+      <c r="P114" s="4" t="s">
         <v>964</v>
       </c>
-      <c r="Q114" s="2" t="s">
+      <c r="Q114" s="4" t="s">
         <v>965</v>
       </c>
     </row>
@@ -8176,52 +8176,52 @@
       <c r="A115" s="1">
         <v>1</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" s="4" t="s">
         <v>966</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="4" t="s">
         <v>967</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D115" s="4" t="s">
         <v>968</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="E115" s="4" t="s">
         <v>969</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="F115" s="4" t="s">
         <v>970</v>
       </c>
-      <c r="G115" s="2" t="s">
+      <c r="G115" s="4" t="s">
         <v>971</v>
       </c>
-      <c r="H115" s="2" t="s">
+      <c r="H115" s="4" t="s">
         <v>972</v>
       </c>
-      <c r="I115" s="2" t="s">
+      <c r="I115" s="4" t="s">
         <v>973</v>
       </c>
-      <c r="J115" s="2" t="s">
+      <c r="J115" s="4" t="s">
         <v>974</v>
       </c>
-      <c r="K115" s="2" t="s">
+      <c r="K115" s="4" t="s">
         <v>975</v>
       </c>
-      <c r="L115" s="2" t="s">
+      <c r="L115" s="4" t="s">
         <v>976</v>
       </c>
-      <c r="M115" s="2" t="s">
+      <c r="M115" s="4" t="s">
         <v>977</v>
       </c>
-      <c r="N115" s="2" t="s">
+      <c r="N115" s="4" t="s">
         <v>978</v>
       </c>
-      <c r="O115" s="2" t="s">
+      <c r="O115" s="4" t="s">
         <v>979</v>
       </c>
-      <c r="P115" s="2" t="s">
+      <c r="P115" s="4" t="s">
         <v>980</v>
       </c>
-      <c r="Q115" s="2" t="s">
+      <c r="Q115" s="4" t="s">
         <v>981</v>
       </c>
     </row>
@@ -8229,52 +8229,52 @@
       <c r="A116" s="1">
         <v>2</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="4" t="s">
         <v>982</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="4" t="s">
         <v>983</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="D116" s="4" t="s">
         <v>984</v>
       </c>
-      <c r="E116" s="2" t="s">
+      <c r="E116" s="4" t="s">
         <v>985</v>
       </c>
-      <c r="F116" s="2" t="s">
+      <c r="F116" s="4" t="s">
         <v>986</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="G116" s="4" t="s">
         <v>987</v>
       </c>
-      <c r="H116" s="2" t="s">
+      <c r="H116" s="4" t="s">
         <v>988</v>
       </c>
-      <c r="I116" s="2" t="s">
+      <c r="I116" s="4" t="s">
         <v>989</v>
       </c>
-      <c r="J116" s="2" t="s">
+      <c r="J116" s="4" t="s">
         <v>990</v>
       </c>
-      <c r="K116" s="2" t="s">
+      <c r="K116" s="4" t="s">
         <v>991</v>
       </c>
-      <c r="L116" s="2" t="s">
+      <c r="L116" s="4" t="s">
         <v>992</v>
       </c>
-      <c r="M116" s="2" t="s">
+      <c r="M116" s="4" t="s">
         <v>993</v>
       </c>
-      <c r="N116" s="2" t="s">
+      <c r="N116" s="4" t="s">
         <v>994</v>
       </c>
-      <c r="O116" s="2" t="s">
+      <c r="O116" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="P116" s="2" t="s">
+      <c r="P116" s="4" t="s">
         <v>996</v>
       </c>
-      <c r="Q116" s="2" t="s">
+      <c r="Q116" s="4" t="s">
         <v>997</v>
       </c>
     </row>
@@ -8282,52 +8282,52 @@
       <c r="A117" s="1">
         <v>3</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="4" t="s">
         <v>998</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="4" t="s">
         <v>999</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="D117" s="4" t="s">
         <v>1000</v>
       </c>
-      <c r="E117" s="2" t="s">
+      <c r="E117" s="4" t="s">
         <v>1001</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="F117" s="4" t="s">
         <v>1002</v>
       </c>
-      <c r="G117" s="2" t="s">
+      <c r="G117" s="4" t="s">
         <v>1003</v>
       </c>
-      <c r="H117" s="2" t="s">
+      <c r="H117" s="4" t="s">
         <v>1004</v>
       </c>
-      <c r="I117" s="2" t="s">
+      <c r="I117" s="4" t="s">
         <v>1005</v>
       </c>
-      <c r="J117" s="2" t="s">
+      <c r="J117" s="4" t="s">
         <v>1006</v>
       </c>
-      <c r="K117" s="2" t="s">
+      <c r="K117" s="4" t="s">
         <v>1007</v>
       </c>
-      <c r="L117" s="2" t="s">
+      <c r="L117" s="4" t="s">
         <v>1008</v>
       </c>
-      <c r="M117" s="2" t="s">
+      <c r="M117" s="4" t="s">
         <v>1009</v>
       </c>
-      <c r="N117" s="2" t="s">
+      <c r="N117" s="4" t="s">
         <v>1010</v>
       </c>
-      <c r="O117" s="2" t="s">
+      <c r="O117" s="4" t="s">
         <v>1011</v>
       </c>
-      <c r="P117" s="2" t="s">
+      <c r="P117" s="4" t="s">
         <v>1012</v>
       </c>
-      <c r="Q117" s="2" t="s">
+      <c r="Q117" s="4" t="s">
         <v>1013</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code emitting for ALU operations is implemented and tested.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -3885,8 +3885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I100" sqref="I100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3984,7 +3984,7 @@
       <c r="J4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -4037,7 +4037,7 @@
       <c r="J5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -4090,7 +4090,7 @@
       <c r="J6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -4143,7 +4143,7 @@
       <c r="J7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="4" t="s">
         <v>63</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -4381,52 +4381,52 @@
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="4" t="s">
         <v>149</v>
       </c>
     </row>
@@ -4434,52 +4434,52 @@
       <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="4" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4487,52 +4487,52 @@
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N14" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="P14" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q14" s="4" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4540,52 +4540,52 @@
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="N15" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="P15" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="Q15" s="4" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4611,7 +4611,7 @@
       <c r="G16" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="4" t="s">
         <v>204</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -4633,7 +4633,7 @@
       <c r="O16" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="P16" s="4" t="s">
         <v>211</v>
       </c>
       <c r="Q16" s="2" t="s">
@@ -4662,7 +4662,7 @@
       <c r="G17" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="4" t="s">
         <v>219</v>
       </c>
       <c r="I17" s="2" t="s">
@@ -4684,7 +4684,7 @@
         <v>225</v>
       </c>
       <c r="O17" s="2"/>
-      <c r="P17" s="2" t="s">
+      <c r="P17" s="4" t="s">
         <v>226</v>
       </c>
       <c r="Q17" s="2" t="s">
@@ -4713,7 +4713,7 @@
       <c r="G18" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="4" t="s">
         <v>234</v>
       </c>
       <c r="I18" s="2" t="s">
@@ -4735,7 +4735,7 @@
         <v>240</v>
       </c>
       <c r="O18" s="2"/>
-      <c r="P18" s="2" t="s">
+      <c r="P18" s="4" t="s">
         <v>241</v>
       </c>
       <c r="Q18" s="2" t="s">
@@ -4764,7 +4764,7 @@
       <c r="G19" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="4" t="s">
         <v>249</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -4786,7 +4786,7 @@
         <v>255</v>
       </c>
       <c r="O19" s="2"/>
-      <c r="P19" s="2" t="s">
+      <c r="P19" s="4" t="s">
         <v>256</v>
       </c>
       <c r="Q19" s="2" t="s">
@@ -4859,7 +4859,7 @@
       <c r="C24" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="4" t="s">
         <v>262</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -4883,7 +4883,7 @@
       <c r="K24" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="L24" s="4" t="s">
         <v>270</v>
       </c>
       <c r="M24" s="2" t="s">
@@ -4912,7 +4912,7 @@
       <c r="C25" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="4" t="s">
         <v>277</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -4936,7 +4936,7 @@
       <c r="K25" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="L25" s="4" t="s">
         <v>283</v>
       </c>
       <c r="M25" s="2" t="s">
@@ -4965,7 +4965,7 @@
       <c r="C26" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="4" t="s">
         <v>289</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -4989,7 +4989,7 @@
       <c r="K26" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L26" s="4" t="s">
         <v>293</v>
       </c>
       <c r="M26" s="2" t="s">
@@ -5018,7 +5018,7 @@
       <c r="C27" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="4" t="s">
         <v>297</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -5040,7 +5040,7 @@
       <c r="K27" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="L27" s="4" t="s">
         <v>301</v>
       </c>
       <c r="M27" s="2" t="s">
@@ -6104,7 +6104,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
-      <c r="K54" s="2" t="s">
+      <c r="K54" s="4" t="s">
         <v>577</v>
       </c>
       <c r="L54" s="2"/>
@@ -6127,7 +6127,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
-      <c r="K55" s="2" t="s">
+      <c r="K55" s="4" t="s">
         <v>578</v>
       </c>
       <c r="L55" s="2"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
-      <c r="K56" s="2" t="s">
+      <c r="K56" s="4" t="s">
         <v>585</v>
       </c>
       <c r="L56" s="2" t="s">
@@ -6201,7 +6201,7 @@
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-      <c r="K57" s="2" t="s">
+      <c r="K57" s="4" t="s">
         <v>594</v>
       </c>
       <c r="L57" s="2"/>
@@ -6379,13 +6379,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-      <c r="F62" s="2" t="s">
+      <c r="F62" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G62" s="4" t="s">
         <v>634</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H62" s="4" t="s">
         <v>635</v>
       </c>
       <c r="I62" s="2"/>
@@ -6393,13 +6393,13 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
-      <c r="N62" s="2" t="s">
+      <c r="N62" s="4" t="s">
         <v>636</v>
       </c>
-      <c r="O62" s="2" t="s">
+      <c r="O62" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="P62" s="2" t="s">
+      <c r="P62" s="4" t="s">
         <v>638</v>
       </c>
       <c r="Q62" s="2"/>
@@ -6412,13 +6412,13 @@
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G63" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="H63" s="4" t="s">
         <v>641</v>
       </c>
       <c r="I63" s="2"/>
@@ -6426,13 +6426,13 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
-      <c r="N63" s="2" t="s">
+      <c r="N63" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="O63" s="2" t="s">
+      <c r="O63" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="P63" s="2" t="s">
+      <c r="P63" s="4" t="s">
         <v>644</v>
       </c>
       <c r="Q63" s="2"/>
@@ -6445,13 +6445,13 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="2" t="s">
+      <c r="F64" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="H64" s="4" t="s">
         <v>647</v>
       </c>
       <c r="I64" s="2"/>
@@ -6459,13 +6459,13 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
-      <c r="N64" s="2" t="s">
+      <c r="N64" s="4" t="s">
         <v>648</v>
       </c>
-      <c r="O64" s="2" t="s">
+      <c r="O64" s="4" t="s">
         <v>649</v>
       </c>
-      <c r="P64" s="2" t="s">
+      <c r="P64" s="4" t="s">
         <v>650</v>
       </c>
       <c r="Q64" s="2"/>
@@ -6478,13 +6478,13 @@
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="4" t="s">
         <v>652</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H65" s="4" t="s">
         <v>653</v>
       </c>
       <c r="I65" s="2"/>
@@ -6492,13 +6492,13 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="2" t="s">
+      <c r="N65" s="4" t="s">
         <v>654</v>
       </c>
-      <c r="O65" s="2" t="s">
+      <c r="O65" s="4" t="s">
         <v>655</v>
       </c>
-      <c r="P65" s="2" t="s">
+      <c r="P65" s="4" t="s">
         <v>656</v>
       </c>
       <c r="Q65" s="2"/>
@@ -7570,7 +7570,7 @@
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
-      <c r="K94" s="2" t="s">
+      <c r="K94" s="4" t="s">
         <v>864</v>
       </c>
       <c r="L94" s="2"/>
@@ -7593,7 +7593,7 @@
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
-      <c r="K95" s="2" t="s">
+      <c r="K95" s="4" t="s">
         <v>865</v>
       </c>
       <c r="L95" s="2"/>
@@ -7628,7 +7628,7 @@
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
-      <c r="K96" s="2" t="s">
+      <c r="K96" s="4" t="s">
         <v>872</v>
       </c>
       <c r="L96" s="2" t="s">
@@ -7667,7 +7667,7 @@
       </c>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
-      <c r="K97" s="2" t="s">
+      <c r="K97" s="4" t="s">
         <v>881</v>
       </c>
       <c r="L97" s="2"/>
@@ -7845,13 +7845,13 @@
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
-      <c r="F102" s="2" t="s">
+      <c r="F102" s="4" t="s">
         <v>920</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="G102" s="4" t="s">
         <v>921</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="H102" s="4" t="s">
         <v>922</v>
       </c>
       <c r="I102" s="2"/>
@@ -7859,13 +7859,13 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
-      <c r="N102" s="2" t="s">
+      <c r="N102" s="4" t="s">
         <v>923</v>
       </c>
-      <c r="O102" s="2" t="s">
+      <c r="O102" s="4" t="s">
         <v>924</v>
       </c>
-      <c r="P102" s="2" t="s">
+      <c r="P102" s="4" t="s">
         <v>925</v>
       </c>
       <c r="Q102" s="2"/>
@@ -7878,13 +7878,13 @@
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
-      <c r="F103" s="2" t="s">
+      <c r="F103" s="4" t="s">
         <v>926</v>
       </c>
-      <c r="G103" s="2" t="s">
+      <c r="G103" s="4" t="s">
         <v>927</v>
       </c>
-      <c r="H103" s="2" t="s">
+      <c r="H103" s="4" t="s">
         <v>928</v>
       </c>
       <c r="I103" s="2"/>
@@ -7892,13 +7892,13 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
-      <c r="N103" s="2" t="s">
+      <c r="N103" s="4" t="s">
         <v>929</v>
       </c>
-      <c r="O103" s="2" t="s">
+      <c r="O103" s="4" t="s">
         <v>930</v>
       </c>
-      <c r="P103" s="2" t="s">
+      <c r="P103" s="4" t="s">
         <v>931</v>
       </c>
       <c r="Q103" s="2"/>
@@ -7911,13 +7911,13 @@
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
-      <c r="F104" s="2" t="s">
+      <c r="F104" s="4" t="s">
         <v>932</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="G104" s="4" t="s">
         <v>933</v>
       </c>
-      <c r="H104" s="2" t="s">
+      <c r="H104" s="4" t="s">
         <v>934</v>
       </c>
       <c r="I104" s="2"/>
@@ -7925,13 +7925,13 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
-      <c r="N104" s="2" t="s">
+      <c r="N104" s="4" t="s">
         <v>935</v>
       </c>
-      <c r="O104" s="2" t="s">
+      <c r="O104" s="4" t="s">
         <v>936</v>
       </c>
-      <c r="P104" s="2" t="s">
+      <c r="P104" s="4" t="s">
         <v>937</v>
       </c>
       <c r="Q104" s="2"/>
@@ -7944,13 +7944,13 @@
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
-      <c r="F105" s="2" t="s">
+      <c r="F105" s="4" t="s">
         <v>938</v>
       </c>
-      <c r="G105" s="2" t="s">
+      <c r="G105" s="4" t="s">
         <v>939</v>
       </c>
-      <c r="H105" s="2" t="s">
+      <c r="H105" s="4" t="s">
         <v>940</v>
       </c>
       <c r="I105" s="2"/>
@@ -7958,13 +7958,13 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
-      <c r="N105" s="2" t="s">
+      <c r="N105" s="4" t="s">
         <v>941</v>
       </c>
-      <c r="O105" s="2" t="s">
+      <c r="O105" s="4" t="s">
         <v>942</v>
       </c>
-      <c r="P105" s="2" t="s">
+      <c r="P105" s="4" t="s">
         <v>943</v>
       </c>
       <c r="Q105" s="2"/>

</xml_diff>

<commit_message>
All register-to-register LD operations emit proper code.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -3559,7 +3559,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3567,6 +3567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -3885,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4169,52 +4170,52 @@
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="N8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="4" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4222,52 +4223,52 @@
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="N9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q9" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4275,52 +4276,52 @@
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="N10" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4328,52 +4329,52 @@
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="N11" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P11" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="4" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4773,7 +4774,7 @@
       <c r="J19" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="4" t="s">
         <v>252</v>
       </c>
       <c r="L19" s="2" t="s">
@@ -6281,52 +6282,52 @@
       <c r="A60" s="1">
         <v>6</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="4" t="s">
         <v>608</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="4" t="s">
         <v>612</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="I60" s="2" t="s">
+      <c r="I60" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="J60" s="2" t="s">
+      <c r="J60" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="K60" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="L60" s="2" t="s">
+      <c r="L60" s="4" t="s">
         <v>617</v>
       </c>
-      <c r="M60" s="2" t="s">
+      <c r="M60" s="4" t="s">
         <v>618</v>
       </c>
-      <c r="N60" s="2" t="s">
+      <c r="N60" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="O60" s="2" t="s">
+      <c r="O60" s="4" t="s">
         <v>620</v>
       </c>
       <c r="P60" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="Q60" s="2" t="s">
+      <c r="Q60" s="4" t="s">
         <v>622</v>
       </c>
     </row>
@@ -6587,7 +6588,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
-      <c r="K69" s="2" t="s">
+      <c r="K69" s="4" t="s">
         <v>661</v>
       </c>
       <c r="L69" s="2"/>
@@ -7747,52 +7748,52 @@
       <c r="A100" s="1">
         <v>6</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="4" t="s">
         <v>894</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="4" t="s">
         <v>895</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D100" s="4" t="s">
         <v>896</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="E100" s="4" t="s">
         <v>897</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F100" s="4" t="s">
         <v>898</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="G100" s="4" t="s">
         <v>899</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>900</v>
       </c>
-      <c r="I100" s="2" t="s">
+      <c r="I100" s="4" t="s">
         <v>901</v>
       </c>
-      <c r="J100" s="2" t="s">
+      <c r="J100" s="4" t="s">
         <v>902</v>
       </c>
-      <c r="K100" s="2" t="s">
+      <c r="K100" s="4" t="s">
         <v>903</v>
       </c>
-      <c r="L100" s="2" t="s">
+      <c r="L100" s="4" t="s">
         <v>904</v>
       </c>
-      <c r="M100" s="2" t="s">
+      <c r="M100" s="4" t="s">
         <v>905</v>
       </c>
-      <c r="N100" s="2" t="s">
+      <c r="N100" s="4" t="s">
         <v>906</v>
       </c>
-      <c r="O100" s="2" t="s">
+      <c r="O100" s="4" t="s">
         <v>907</v>
       </c>
       <c r="P100" s="2" t="s">
         <v>908</v>
       </c>
-      <c r="Q100" s="2" t="s">
+      <c r="Q100" s="4" t="s">
         <v>909</v>
       </c>
     </row>
@@ -8053,7 +8054,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
-      <c r="K109" s="2" t="s">
+      <c r="K109" s="4" t="s">
         <v>948</v>
       </c>
       <c r="L109" s="2"/>

</xml_diff>

<commit_message>
All LD operations now emit proper code.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -3886,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K109" sqref="K109"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,10 +3961,10 @@
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -3976,7 +3976,7 @@
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -3988,7 +3988,7 @@
       <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -4000,7 +4000,7 @@
       <c r="O4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q4" s="4" t="s">
@@ -4014,10 +4014,10 @@
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -4029,7 +4029,7 @@
       <c r="G5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -4041,7 +4041,7 @@
       <c r="K5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M5" s="4" t="s">
@@ -4053,7 +4053,7 @@
       <c r="O5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="4" t="s">
         <v>36</v>
       </c>
       <c r="Q5" s="4" t="s">
@@ -4067,10 +4067,10 @@
       <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -4082,7 +4082,7 @@
       <c r="G6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -4094,7 +4094,7 @@
       <c r="K6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="4" t="s">
         <v>48</v>
       </c>
       <c r="M6" s="4" t="s">
@@ -4106,7 +4106,7 @@
       <c r="O6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="4" t="s">
         <v>52</v>
       </c>
       <c r="Q6" s="4" t="s">
@@ -4120,10 +4120,10 @@
       <c r="B7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -4135,7 +4135,7 @@
       <c r="G7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="4" t="s">
         <v>60</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -4147,7 +4147,7 @@
       <c r="K7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="4" t="s">
         <v>64</v>
       </c>
       <c r="M7" s="4" t="s">
@@ -4159,7 +4159,7 @@
       <c r="O7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="4" t="s">
         <v>68</v>
       </c>
       <c r="Q7" s="4" t="s">
@@ -4863,7 +4863,7 @@
       <c r="D24" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="4" t="s">
         <v>263</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -4875,7 +4875,7 @@
       <c r="H24" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="4" t="s">
         <v>267</v>
       </c>
       <c r="J24" s="4" t="s">
@@ -4887,7 +4887,7 @@
       <c r="L24" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="M24" s="4" t="s">
         <v>271</v>
       </c>
       <c r="N24" s="4" t="s">
@@ -4899,7 +4899,7 @@
       <c r="P24" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="Q24" s="4" t="s">
         <v>274</v>
       </c>
     </row>
@@ -4916,7 +4916,7 @@
       <c r="D25" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="4" t="s">
         <v>278</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -4928,7 +4928,7 @@
       <c r="H25" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="4" t="s">
         <v>280</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -4940,7 +4940,7 @@
       <c r="L25" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="M25" s="4" t="s">
         <v>284</v>
       </c>
       <c r="N25" s="4" t="s">
@@ -4952,7 +4952,7 @@
       <c r="P25" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="Q25" s="2" t="s">
+      <c r="Q25" s="4" t="s">
         <v>286</v>
       </c>
     </row>
@@ -4969,7 +4969,7 @@
       <c r="D26" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -4993,7 +4993,7 @@
       <c r="L26" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="M26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="N26" s="4" t="s">
@@ -5022,7 +5022,7 @@
       <c r="D27" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="4" t="s">
         <v>298</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -5044,7 +5044,7 @@
       <c r="L27" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="4" t="s">
         <v>302</v>
       </c>
       <c r="N27" s="4" t="s">
@@ -6143,10 +6143,10 @@
         <v>2</v>
       </c>
       <c r="B56" s="2"/>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="4" t="s">
         <v>580</v>
       </c>
       <c r="E56" s="4" t="s">
@@ -6158,7 +6158,7 @@
       <c r="G56" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="4" t="s">
         <v>584</v>
       </c>
       <c r="I56" s="2"/>
@@ -6166,7 +6166,7 @@
       <c r="K56" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="L56" s="2" t="s">
+      <c r="L56" s="4" t="s">
         <v>586</v>
       </c>
       <c r="M56" s="4" t="s">
@@ -6178,7 +6178,7 @@
       <c r="O56" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="P56" s="2" t="s">
+      <c r="P56" s="4" t="s">
         <v>590</v>
       </c>
       <c r="Q56" s="2"/>
@@ -6220,13 +6220,13 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="H58" s="4" t="s">
         <v>597</v>
       </c>
       <c r="I58" s="2"/>
@@ -6234,13 +6234,13 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
-      <c r="N58" s="2" t="s">
+      <c r="N58" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="O58" s="2" t="s">
+      <c r="O58" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="P58" s="2" t="s">
+      <c r="P58" s="4" t="s">
         <v>600</v>
       </c>
       <c r="Q58" s="2"/>
@@ -6253,13 +6253,13 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="4" t="s">
         <v>603</v>
       </c>
       <c r="I59" s="2"/>
@@ -6267,13 +6267,13 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
-      <c r="N59" s="2" t="s">
+      <c r="N59" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="O59" s="2" t="s">
+      <c r="O59" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="P59" s="2" t="s">
+      <c r="P59" s="4" t="s">
         <v>606</v>
       </c>
       <c r="Q59" s="2"/>
@@ -6300,7 +6300,7 @@
       <c r="G60" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H60" s="4" t="s">
         <v>613</v>
       </c>
       <c r="I60" s="4" t="s">
@@ -6324,7 +6324,7 @@
       <c r="O60" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="P60" s="2" t="s">
+      <c r="P60" s="4" t="s">
         <v>621</v>
       </c>
       <c r="Q60" s="4" t="s">
@@ -6335,39 +6335,39 @@
       <c r="A61" s="1">
         <v>7</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="4" t="s">
         <v>626</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F61" s="4" t="s">
         <v>627</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G61" s="4" t="s">
         <v>628</v>
       </c>
       <c r="H61" s="2"/>
-      <c r="I61" s="2" t="s">
+      <c r="I61" s="4" t="s">
         <v>629</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
-      <c r="N61" s="2" t="s">
+      <c r="N61" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="O61" s="2" t="s">
+      <c r="O61" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="P61" s="2" t="s">
+      <c r="P61" s="4" t="s">
         <v>632</v>
       </c>
       <c r="Q61" s="2"/>
@@ -7609,10 +7609,10 @@
         <v>2</v>
       </c>
       <c r="B96" s="2"/>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="4" t="s">
         <v>866</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D96" s="4" t="s">
         <v>867</v>
       </c>
       <c r="E96" s="4" t="s">
@@ -7624,7 +7624,7 @@
       <c r="G96" s="4" t="s">
         <v>870</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="H96" s="4" t="s">
         <v>871</v>
       </c>
       <c r="I96" s="2"/>
@@ -7632,7 +7632,7 @@
       <c r="K96" s="4" t="s">
         <v>872</v>
       </c>
-      <c r="L96" s="2" t="s">
+      <c r="L96" s="4" t="s">
         <v>873</v>
       </c>
       <c r="M96" s="4" t="s">
@@ -7644,7 +7644,7 @@
       <c r="O96" s="4" t="s">
         <v>876</v>
       </c>
-      <c r="P96" s="2" t="s">
+      <c r="P96" s="4" t="s">
         <v>877</v>
       </c>
       <c r="Q96" s="2"/>
@@ -7686,13 +7686,13 @@
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
-      <c r="F98" s="2" t="s">
+      <c r="F98" s="4" t="s">
         <v>882</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G98" s="4" t="s">
         <v>883</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="H98" s="4" t="s">
         <v>884</v>
       </c>
       <c r="I98" s="2"/>
@@ -7700,13 +7700,13 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
-      <c r="N98" s="2" t="s">
+      <c r="N98" s="4" t="s">
         <v>885</v>
       </c>
-      <c r="O98" s="2" t="s">
+      <c r="O98" s="4" t="s">
         <v>886</v>
       </c>
-      <c r="P98" s="2" t="s">
+      <c r="P98" s="4" t="s">
         <v>887</v>
       </c>
       <c r="Q98" s="2"/>
@@ -7719,13 +7719,13 @@
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
-      <c r="F99" s="2" t="s">
+      <c r="F99" s="4" t="s">
         <v>888</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="G99" s="4" t="s">
         <v>889</v>
       </c>
-      <c r="H99" s="2" t="s">
+      <c r="H99" s="4" t="s">
         <v>890</v>
       </c>
       <c r="I99" s="2"/>
@@ -7733,13 +7733,13 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
-      <c r="N99" s="2" t="s">
+      <c r="N99" s="4" t="s">
         <v>891</v>
       </c>
-      <c r="O99" s="2" t="s">
+      <c r="O99" s="4" t="s">
         <v>892</v>
       </c>
-      <c r="P99" s="2" t="s">
+      <c r="P99" s="4" t="s">
         <v>893</v>
       </c>
       <c r="Q99" s="2"/>
@@ -7766,7 +7766,7 @@
       <c r="G100" s="4" t="s">
         <v>899</v>
       </c>
-      <c r="H100" s="2" t="s">
+      <c r="H100" s="4" t="s">
         <v>900</v>
       </c>
       <c r="I100" s="4" t="s">
@@ -7790,7 +7790,7 @@
       <c r="O100" s="4" t="s">
         <v>907</v>
       </c>
-      <c r="P100" s="2" t="s">
+      <c r="P100" s="4" t="s">
         <v>908</v>
       </c>
       <c r="Q100" s="4" t="s">
@@ -7801,39 +7801,39 @@
       <c r="A101" s="1">
         <v>7</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="4" t="s">
         <v>910</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="4" t="s">
         <v>911</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D101" s="4" t="s">
         <v>912</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E101" s="4" t="s">
         <v>913</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F101" s="4" t="s">
         <v>914</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="G101" s="4" t="s">
         <v>915</v>
       </c>
       <c r="H101" s="2"/>
-      <c r="I101" s="2" t="s">
+      <c r="I101" s="4" t="s">
         <v>916</v>
       </c>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
-      <c r="N101" s="2" t="s">
+      <c r="N101" s="4" t="s">
         <v>917</v>
       </c>
-      <c r="O101" s="2" t="s">
+      <c r="O101" s="4" t="s">
         <v>918</v>
       </c>
-      <c r="P101" s="2" t="s">
+      <c r="P101" s="4" t="s">
         <v>919</v>
       </c>
       <c r="Q101" s="2"/>

</xml_diff>

<commit_message>
Control flow code emitting implementation is in progress.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -3886,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4011,7 +4011,7 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -4615,7 +4615,7 @@
       <c r="H16" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="4" t="s">
         <v>205</v>
       </c>
       <c r="J16" s="2" t="s">
@@ -4637,7 +4637,7 @@
       <c r="P16" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="Q16" s="4" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4666,7 +4666,7 @@
       <c r="H17" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="4" t="s">
         <v>220</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -4688,7 +4688,7 @@
       <c r="P17" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="Q17" s="4" t="s">
         <v>227</v>
       </c>
     </row>
@@ -4717,7 +4717,7 @@
       <c r="H18" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="4" t="s">
         <v>235</v>
       </c>
       <c r="J18" s="2" t="s">
@@ -4739,7 +4739,7 @@
       <c r="P18" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="Q18" s="4" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4768,7 +4768,7 @@
       <c r="H19" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="4" t="s">
         <v>250</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -4790,7 +4790,7 @@
       <c r="P19" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="Q19" s="4" t="s">
         <v>257</v>
       </c>
     </row>
@@ -6197,7 +6197,7 @@
       <c r="G57" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="4" t="s">
         <v>593</v>
       </c>
       <c r="I57" s="2"/>
@@ -7663,7 +7663,7 @@
       <c r="G97" s="4" t="s">
         <v>879</v>
       </c>
-      <c r="H97" s="2" t="s">
+      <c r="H97" s="4" t="s">
         <v>880</v>
       </c>
       <c r="I97" s="2"/>

</xml_diff>

<commit_message>
Now all Z80 operations emit proper code.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -3887,7 +3887,7 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4035,7 +4035,7 @@
       <c r="I5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -4064,7 +4064,7 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -4088,7 +4088,7 @@
       <c r="I6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="4" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -4117,7 +4117,7 @@
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -4141,7 +4141,7 @@
       <c r="I7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="4" t="s">
         <v>62</v>
       </c>
       <c r="K7" s="4" t="s">
@@ -4594,19 +4594,19 @@
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>198</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="4" t="s">
         <v>202</v>
       </c>
       <c r="G16" s="4" t="s">
@@ -4618,20 +4618,20 @@
       <c r="I16" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="4" t="s">
         <v>206</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="4" t="s">
         <v>208</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="N16" s="2" t="s">
+      <c r="N16" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O16" s="4" t="s">
         <v>210</v>
       </c>
       <c r="P16" s="4" t="s">
@@ -4645,19 +4645,19 @@
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>213</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>215</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="4" t="s">
         <v>217</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -4669,19 +4669,19 @@
       <c r="I17" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="4" t="s">
         <v>221</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="4" t="s">
         <v>223</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="N17" s="4" t="s">
         <v>225</v>
       </c>
       <c r="O17" s="2"/>
@@ -4696,19 +4696,19 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>228</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>230</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="4" t="s">
         <v>232</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -4720,19 +4720,19 @@
       <c r="I18" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="4" t="s">
         <v>238</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="N18" s="4" t="s">
         <v>240</v>
       </c>
       <c r="O18" s="2"/>
@@ -4747,19 +4747,19 @@
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>243</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="4" t="s">
         <v>245</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="4" t="s">
         <v>247</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -4771,19 +4771,19 @@
       <c r="I19" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="4" t="s">
         <v>251</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="4" t="s">
         <v>253</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="N19" s="4" t="s">
         <v>255</v>
       </c>
       <c r="O19" s="2"/>
@@ -6565,7 +6565,7 @@
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
-      <c r="K68" s="2" t="s">
+      <c r="K68" s="4" t="s">
         <v>660</v>
       </c>
       <c r="L68" s="2"/>
@@ -8031,7 +8031,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
-      <c r="K108" s="2" t="s">
+      <c r="K108" s="4" t="s">
         <v>947</v>
       </c>
       <c r="L108" s="2"/>

</xml_diff>

<commit_message>
Stack operations emit proper operation code with the lightweight parser.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -8979,8 +8979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114:Q129"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9690,7 +9690,7 @@
       <c r="B16" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>199</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -9702,7 +9702,7 @@
       <c r="F16" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>203</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -9741,7 +9741,7 @@
       <c r="B17" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>214</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -9753,7 +9753,7 @@
       <c r="F17" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="4" t="s">
         <v>218</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -9792,7 +9792,7 @@
       <c r="B18" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>229</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -9804,7 +9804,7 @@
       <c r="F18" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="4" t="s">
         <v>233</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -9843,7 +9843,7 @@
       <c r="B19" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>244</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -9855,7 +9855,7 @@
       <c r="F19" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="4" t="s">
         <v>248</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -9965,7 +9965,7 @@
       <c r="G24" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="4" t="s">
         <v>266</v>
       </c>
       <c r="I24" s="2" t="s">
@@ -9989,7 +9989,7 @@
       <c r="O24" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="P24" s="4" t="s">
         <v>273</v>
       </c>
       <c r="Q24" s="2" t="s">
@@ -10018,7 +10018,7 @@
       <c r="G25" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="4" t="s">
         <v>279</v>
       </c>
       <c r="I25" s="2" t="s">
@@ -10042,7 +10042,7 @@
       <c r="O25" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="P25" s="2" t="s">
+      <c r="P25" s="4" t="s">
         <v>285</v>
       </c>
       <c r="Q25" s="2" t="s">
@@ -10071,7 +10071,7 @@
       <c r="G26" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="4" t="s">
         <v>266</v>
       </c>
       <c r="I26" s="4" t="s">
@@ -10095,7 +10095,7 @@
       <c r="O26" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="P26" s="4" t="s">
         <v>273</v>
       </c>
       <c r="Q26" s="4" t="s">
@@ -10124,7 +10124,7 @@
       <c r="G27" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="4" t="s">
         <v>279</v>
       </c>
       <c r="I27" s="2"/>
@@ -10146,7 +10146,7 @@
       <c r="O27" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="P27" s="2" t="s">
+      <c r="P27" s="4" t="s">
         <v>285</v>
       </c>
       <c r="Q27" s="2"/>
@@ -11644,7 +11644,7 @@
         <v>4</v>
       </c>
       <c r="B68" s="2"/>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="4" t="s">
         <v>657</v>
       </c>
       <c r="D68" s="2"/>
@@ -11652,7 +11652,7 @@
         <v>658</v>
       </c>
       <c r="F68" s="2"/>
-      <c r="G68" s="2" t="s">
+      <c r="G68" s="4" t="s">
         <v>659</v>
       </c>
       <c r="H68" s="2"/>
@@ -13110,7 +13110,7 @@
         <v>4</v>
       </c>
       <c r="B108" s="2"/>
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="4" t="s">
         <v>944</v>
       </c>
       <c r="D108" s="2"/>
@@ -13118,7 +13118,7 @@
         <v>945</v>
       </c>
       <c r="F108" s="2"/>
-      <c r="G108" s="2" t="s">
+      <c r="G108" s="4" t="s">
         <v>946</v>
       </c>
       <c r="H108" s="2"/>

</xml_diff>

<commit_message>
Control flow operation code emitting is being refactored.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -8979,8 +8979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G108" sqref="G108"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16:Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9708,7 +9708,7 @@
       <c r="H16" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="4" t="s">
         <v>205</v>
       </c>
       <c r="J16" s="2" t="s">
@@ -9730,7 +9730,7 @@
       <c r="P16" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="Q16" s="4" t="s">
         <v>212</v>
       </c>
     </row>
@@ -9759,7 +9759,7 @@
       <c r="H17" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="4" t="s">
         <v>220</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -9781,7 +9781,7 @@
       <c r="P17" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="Q17" s="4" t="s">
         <v>227</v>
       </c>
     </row>
@@ -9810,7 +9810,7 @@
       <c r="H18" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="4" t="s">
         <v>235</v>
       </c>
       <c r="J18" s="2" t="s">
@@ -9832,7 +9832,7 @@
       <c r="P18" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="Q18" s="4" t="s">
         <v>242</v>
       </c>
     </row>
@@ -9861,7 +9861,7 @@
       <c r="H19" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="4" t="s">
         <v>250</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -9883,7 +9883,7 @@
       <c r="P19" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="Q19" s="4" t="s">
         <v>257</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Increment and decrement operations refactored.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -8980,7 +8980,7 @@
   <dimension ref="A1:Q129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16:Q19"/>
+      <selection activeCell="M96" sqref="M96:O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9060,13 +9060,13 @@
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -9075,7 +9075,7 @@
       <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -9084,13 +9084,13 @@
       <c r="L4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P4" s="2" t="s">
@@ -9104,7 +9104,7 @@
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -9113,13 +9113,13 @@
       <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -9128,7 +9128,7 @@
       <c r="I5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -9137,13 +9137,13 @@
       <c r="L5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="P5" s="2" t="s">
@@ -9157,7 +9157,7 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -9166,13 +9166,13 @@
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -9181,7 +9181,7 @@
       <c r="I6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="4" t="s">
         <v>46</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -9190,13 +9190,13 @@
       <c r="L6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="4" t="s">
         <v>51</v>
       </c>
       <c r="P6" s="2" t="s">
@@ -9210,7 +9210,7 @@
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -9219,13 +9219,13 @@
       <c r="D7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="4" t="s">
         <v>59</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -9234,7 +9234,7 @@
       <c r="I7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="4" t="s">
         <v>62</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -9243,13 +9243,13 @@
       <c r="L7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="4" t="s">
         <v>67</v>
       </c>
       <c r="P7" s="2" t="s">
@@ -9687,19 +9687,19 @@
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>198</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="4" t="s">
         <v>202</v>
       </c>
       <c r="G16" s="4" t="s">
@@ -9711,20 +9711,20 @@
       <c r="I16" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="4" t="s">
         <v>206</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="4" t="s">
         <v>208</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="N16" s="2" t="s">
+      <c r="N16" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O16" s="4" t="s">
         <v>210</v>
       </c>
       <c r="P16" s="2" t="s">
@@ -9738,19 +9738,19 @@
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>213</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>215</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="4" t="s">
         <v>217</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -9762,19 +9762,19 @@
       <c r="I17" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="4" t="s">
         <v>221</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="4" t="s">
         <v>223</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="N17" s="4" t="s">
         <v>225</v>
       </c>
       <c r="O17" s="2"/>
@@ -9789,19 +9789,19 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>228</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="4" t="s">
         <v>232</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -9813,19 +9813,19 @@
       <c r="I18" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="N18" s="4" t="s">
         <v>240</v>
       </c>
       <c r="O18" s="2"/>
@@ -9840,19 +9840,19 @@
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>243</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="4" t="s">
         <v>245</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="4" t="s">
         <v>247</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -9864,19 +9864,19 @@
       <c r="I19" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="4" t="s">
         <v>251</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="4" t="s">
         <v>253</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="N19" s="4" t="s">
         <v>255</v>
       </c>
       <c r="O19" s="2"/>
@@ -11242,13 +11242,13 @@
       <c r="D56" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G56" s="4" t="s">
         <v>583</v>
       </c>
       <c r="H56" s="2" t="s">
@@ -11262,13 +11262,13 @@
       <c r="L56" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="M56" s="2" t="s">
+      <c r="M56" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="N56" s="2" t="s">
+      <c r="N56" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="O56" s="2" t="s">
+      <c r="O56" s="4" t="s">
         <v>589</v>
       </c>
       <c r="P56" s="2" t="s">
@@ -11284,10 +11284,10 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="G57" s="4" t="s">
         <v>592</v>
       </c>
       <c r="H57" s="2" t="s">
@@ -11648,7 +11648,7 @@
         <v>657</v>
       </c>
       <c r="D68" s="2"/>
-      <c r="E68" s="2" t="s">
+      <c r="E68" s="4" t="s">
         <v>658</v>
       </c>
       <c r="F68" s="2"/>
@@ -11658,7 +11658,7 @@
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
-      <c r="K68" s="2" t="s">
+      <c r="K68" s="4" t="s">
         <v>660</v>
       </c>
       <c r="L68" s="2"/>
@@ -12708,13 +12708,13 @@
       <c r="D96" s="2" t="s">
         <v>867</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="E96" s="4" t="s">
         <v>868</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="F96" s="4" t="s">
         <v>869</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="G96" s="4" t="s">
         <v>870</v>
       </c>
       <c r="H96" s="2" t="s">
@@ -12728,13 +12728,13 @@
       <c r="L96" s="2" t="s">
         <v>873</v>
       </c>
-      <c r="M96" s="2" t="s">
+      <c r="M96" s="4" t="s">
         <v>874</v>
       </c>
-      <c r="N96" s="2" t="s">
+      <c r="N96" s="4" t="s">
         <v>875</v>
       </c>
-      <c r="O96" s="2" t="s">
+      <c r="O96" s="4" t="s">
         <v>876</v>
       </c>
       <c r="P96" s="2" t="s">
@@ -12750,10 +12750,10 @@
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
-      <c r="F97" s="2" t="s">
+      <c r="F97" s="4" t="s">
         <v>878</v>
       </c>
-      <c r="G97" s="2" t="s">
+      <c r="G97" s="4" t="s">
         <v>879</v>
       </c>
       <c r="H97" s="2" t="s">
@@ -13114,7 +13114,7 @@
         <v>944</v>
       </c>
       <c r="D108" s="2"/>
-      <c r="E108" s="2" t="s">
+      <c r="E108" s="4" t="s">
         <v>945</v>
       </c>
       <c r="F108" s="2"/>
@@ -13124,7 +13124,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
-      <c r="K108" s="2" t="s">
+      <c r="K108" s="4" t="s">
         <v>947</v>
       </c>
       <c r="L108" s="2"/>

</xml_diff>

<commit_message>
Bit manipulation operations refactored.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -8979,8 +8979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I91" sqref="I91"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9705,7 +9705,7 @@
       <c r="G16" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="4" t="s">
         <v>204</v>
       </c>
       <c r="I16" s="4" t="s">
@@ -9714,7 +9714,7 @@
       <c r="J16" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="4" t="s">
         <v>207</v>
       </c>
       <c r="L16" s="4" t="s">
@@ -9727,7 +9727,7 @@
       <c r="O16" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="P16" s="4" t="s">
         <v>211</v>
       </c>
       <c r="Q16" s="4" t="s">
@@ -9747,7 +9747,7 @@
       <c r="D17" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="4" t="s">
         <v>216</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -9756,7 +9756,7 @@
       <c r="G17" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="4" t="s">
         <v>219</v>
       </c>
       <c r="I17" s="4" t="s">
@@ -9771,14 +9771,14 @@
       <c r="L17" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="4" t="s">
         <v>224</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>225</v>
       </c>
       <c r="O17" s="2"/>
-      <c r="P17" s="2" t="s">
+      <c r="P17" s="4" t="s">
         <v>226</v>
       </c>
       <c r="Q17" s="4" t="s">
@@ -9807,7 +9807,7 @@
       <c r="G18" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="4" t="s">
         <v>234</v>
       </c>
       <c r="I18" s="4" t="s">
@@ -9829,7 +9829,7 @@
         <v>240</v>
       </c>
       <c r="O18" s="2"/>
-      <c r="P18" s="2" t="s">
+      <c r="P18" s="4" t="s">
         <v>241</v>
       </c>
       <c r="Q18" s="4" t="s">
@@ -9858,7 +9858,7 @@
       <c r="G19" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="4" t="s">
         <v>249</v>
       </c>
       <c r="I19" s="4" t="s">
@@ -9880,7 +9880,7 @@
         <v>255</v>
       </c>
       <c r="O19" s="2"/>
-      <c r="P19" s="2" t="s">
+      <c r="P19" s="4" t="s">
         <v>256</v>
       </c>
       <c r="Q19" s="4" t="s">
@@ -9947,10 +9947,10 @@
       <c r="A24" s="1">
         <v>4</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>261</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -9971,10 +9971,10 @@
       <c r="I24" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="4" t="s">
         <v>269</v>
       </c>
       <c r="L24" s="4" t="s">
@@ -10000,10 +10000,10 @@
       <c r="A25" s="1">
         <v>5</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="4" t="s">
         <v>276</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -10024,10 +10024,10 @@
       <c r="I25" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K25" s="4" t="s">
         <v>282</v>
       </c>
       <c r="L25" s="4" t="s">
@@ -10053,10 +10053,10 @@
       <c r="A26" s="1">
         <v>6</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="4" t="s">
         <v>288</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -10077,10 +10077,10 @@
       <c r="I26" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="4" t="s">
         <v>292</v>
       </c>
       <c r="L26" s="4" t="s">
@@ -10106,10 +10106,10 @@
       <c r="A27" s="1">
         <v>7</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="4" t="s">
         <v>296</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -10128,10 +10128,10 @@
         <v>279</v>
       </c>
       <c r="I27" s="2"/>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="4" t="s">
         <v>300</v>
       </c>
       <c r="L27" s="4" t="s">
@@ -10285,52 +10285,52 @@
       <c r="A34" s="1">
         <v>0</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="K34" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="L34" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="M34" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="N34" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="O34" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="P34" s="2" t="s">
+      <c r="P34" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="Q34" s="2" t="s">
+      <c r="Q34" s="4" t="s">
         <v>335</v>
       </c>
     </row>
@@ -10338,52 +10338,52 @@
       <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="I35" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="K35" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="L35" s="2" t="s">
+      <c r="L35" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="M35" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="N35" s="2" t="s">
+      <c r="N35" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="O35" s="2" t="s">
+      <c r="O35" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="P35" s="2" t="s">
+      <c r="P35" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="Q35" s="2" t="s">
+      <c r="Q35" s="4" t="s">
         <v>351</v>
       </c>
     </row>
@@ -10391,52 +10391,52 @@
       <c r="A36" s="1">
         <v>2</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="I36" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="J36" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="K36" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="L36" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="M36" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="N36" s="2" t="s">
+      <c r="N36" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="O36" s="2" t="s">
+      <c r="O36" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="P36" s="2" t="s">
+      <c r="P36" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="Q36" s="2" t="s">
+      <c r="Q36" s="4" t="s">
         <v>367</v>
       </c>
     </row>
@@ -10444,52 +10444,52 @@
       <c r="A37" s="1">
         <v>3</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="I37" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J37" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="K37" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="L37" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="M37" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="N37" s="2" t="s">
+      <c r="N37" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="O37" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="P37" s="2" t="s">
+      <c r="P37" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="Q37" s="2" t="s">
+      <c r="Q37" s="4" t="s">
         <v>383</v>
       </c>
     </row>
@@ -10497,52 +10497,52 @@
       <c r="A38" s="1">
         <v>4</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="I38" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="K38" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="L38" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="M38" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="N38" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="O38" s="2" t="s">
+      <c r="O38" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="P38" s="2" t="s">
+      <c r="P38" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="Q38" s="2" t="s">
+      <c r="Q38" s="4" t="s">
         <v>399</v>
       </c>
     </row>
@@ -10550,52 +10550,52 @@
       <c r="A39" s="1">
         <v>5</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="K39" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="L39" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="M39" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="N39" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="O39" s="2" t="s">
+      <c r="O39" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="P39" s="2" t="s">
+      <c r="P39" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="Q39" s="2" t="s">
+      <c r="Q39" s="4" t="s">
         <v>415</v>
       </c>
     </row>
@@ -10603,52 +10603,52 @@
       <c r="A40" s="1">
         <v>6</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="K40" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="L40" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="M40" s="2" t="s">
+      <c r="M40" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="N40" s="2" t="s">
+      <c r="N40" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="O40" s="2" t="s">
+      <c r="O40" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="P40" s="2" t="s">
+      <c r="P40" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="Q40" s="2" t="s">
+      <c r="Q40" s="4" t="s">
         <v>431</v>
       </c>
     </row>
@@ -10656,52 +10656,52 @@
       <c r="A41" s="1">
         <v>7</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I41" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="K41" s="2" t="s">
+      <c r="K41" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="L41" s="2" t="s">
+      <c r="L41" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="M41" s="2" t="s">
+      <c r="M41" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="N41" s="2" t="s">
+      <c r="N41" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="O41" s="2" t="s">
+      <c r="O41" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="P41" s="2" t="s">
+      <c r="P41" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="Q41" s="2" t="s">
+      <c r="Q41" s="4" t="s">
         <v>447</v>
       </c>
     </row>
@@ -10709,52 +10709,52 @@
       <c r="A42" s="1">
         <v>8</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="I42" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="J42" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="K42" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="L42" s="2" t="s">
+      <c r="L42" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="M42" s="2" t="s">
+      <c r="M42" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="N42" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="O42" s="2" t="s">
+      <c r="O42" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="P42" s="2" t="s">
+      <c r="P42" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="Q42" s="2" t="s">
+      <c r="Q42" s="4" t="s">
         <v>463</v>
       </c>
     </row>
@@ -10762,52 +10762,52 @@
       <c r="A43" s="1">
         <v>9</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H43" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="I43" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="J43" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="K43" s="2" t="s">
+      <c r="K43" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="L43" s="2" t="s">
+      <c r="L43" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="M43" s="2" t="s">
+      <c r="M43" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="N43" s="2" t="s">
+      <c r="N43" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="O43" s="2" t="s">
+      <c r="O43" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="P43" s="2" t="s">
+      <c r="P43" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="Q43" s="2" t="s">
+      <c r="Q43" s="4" t="s">
         <v>479</v>
       </c>
     </row>
@@ -10815,52 +10815,52 @@
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="I44" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="J44" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="K44" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="L44" s="2" t="s">
+      <c r="L44" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="M44" s="2" t="s">
+      <c r="M44" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="N44" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="O44" s="2" t="s">
+      <c r="O44" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="P44" s="2" t="s">
+      <c r="P44" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="Q44" s="2" t="s">
+      <c r="Q44" s="4" t="s">
         <v>495</v>
       </c>
     </row>
@@ -10868,52 +10868,52 @@
       <c r="A45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H45" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="I45" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="J45" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="K45" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="L45" s="2" t="s">
+      <c r="L45" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="M45" s="2" t="s">
+      <c r="M45" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="N45" s="2" t="s">
+      <c r="N45" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="O45" s="2" t="s">
+      <c r="O45" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="P45" s="2" t="s">
+      <c r="P45" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="Q45" s="2" t="s">
+      <c r="Q45" s="4" t="s">
         <v>511</v>
       </c>
     </row>
@@ -10921,52 +10921,52 @@
       <c r="A46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="I46" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="J46" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="K46" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="L46" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="M46" s="2" t="s">
+      <c r="M46" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="N46" s="2" t="s">
+      <c r="N46" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="O46" s="2" t="s">
+      <c r="O46" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="P46" s="2" t="s">
+      <c r="P46" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="Q46" s="2" t="s">
+      <c r="Q46" s="4" t="s">
         <v>527</v>
       </c>
     </row>
@@ -10974,52 +10974,52 @@
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="I47" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="J47" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="K47" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="L47" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="M47" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="N47" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="O47" s="2" t="s">
+      <c r="O47" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="P47" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="Q47" s="2" t="s">
+      <c r="Q47" s="4" t="s">
         <v>543</v>
       </c>
     </row>
@@ -11027,52 +11027,52 @@
       <c r="A48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I48" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J48" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="K48" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="L48" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="M48" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="N48" s="2" t="s">
+      <c r="N48" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="O48" s="2" t="s">
+      <c r="O48" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="P48" s="2" t="s">
+      <c r="P48" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="Q48" s="2" t="s">
+      <c r="Q48" s="4" t="s">
         <v>559</v>
       </c>
     </row>
@@ -11080,52 +11080,52 @@
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G49" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="I49" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="J49" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="K49" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="L49" s="2" t="s">
+      <c r="L49" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="M49" s="2" t="s">
+      <c r="M49" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="N49" s="2" t="s">
+      <c r="N49" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="O49" s="2" t="s">
+      <c r="O49" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="P49" s="2" t="s">
+      <c r="P49" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="Q49" s="2" t="s">
+      <c r="Q49" s="4" t="s">
         <v>575</v>
       </c>
     </row>
@@ -11473,13 +11473,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-      <c r="F62" s="2" t="s">
+      <c r="F62" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="G62" s="4" t="s">
         <v>634</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H62" s="4" t="s">
         <v>635</v>
       </c>
       <c r="I62" s="2"/>
@@ -11487,13 +11487,13 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
-      <c r="N62" s="2" t="s">
+      <c r="N62" s="4" t="s">
         <v>636</v>
       </c>
-      <c r="O62" s="2" t="s">
+      <c r="O62" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="P62" s="2" t="s">
+      <c r="P62" s="4" t="s">
         <v>638</v>
       </c>
       <c r="Q62" s="2"/>
@@ -11506,13 +11506,13 @@
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G63" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="H63" s="4" t="s">
         <v>641</v>
       </c>
       <c r="I63" s="2"/>
@@ -11520,13 +11520,13 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
-      <c r="N63" s="2" t="s">
+      <c r="N63" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="O63" s="2" t="s">
+      <c r="O63" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="P63" s="2" t="s">
+      <c r="P63" s="4" t="s">
         <v>644</v>
       </c>
       <c r="Q63" s="2"/>
@@ -11539,13 +11539,13 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="2" t="s">
+      <c r="F64" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="H64" s="4" t="s">
         <v>647</v>
       </c>
       <c r="I64" s="2"/>
@@ -11553,13 +11553,13 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
-      <c r="N64" s="2" t="s">
+      <c r="N64" s="4" t="s">
         <v>648</v>
       </c>
-      <c r="O64" s="2" t="s">
+      <c r="O64" s="4" t="s">
         <v>649</v>
       </c>
-      <c r="P64" s="2" t="s">
+      <c r="P64" s="4" t="s">
         <v>650</v>
       </c>
       <c r="Q64" s="2"/>
@@ -11572,13 +11572,13 @@
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="4" t="s">
         <v>652</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H65" s="4" t="s">
         <v>653</v>
       </c>
       <c r="I65" s="2"/>
@@ -11586,13 +11586,13 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="2" t="s">
+      <c r="N65" s="4" t="s">
         <v>654</v>
       </c>
-      <c r="O65" s="2" t="s">
+      <c r="O65" s="4" t="s">
         <v>655</v>
       </c>
-      <c r="P65" s="2" t="s">
+      <c r="P65" s="4" t="s">
         <v>656</v>
       </c>
       <c r="Q65" s="2"/>
@@ -11751,52 +11751,52 @@
       <c r="A74" s="1">
         <v>0</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E74" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="H74" s="4" t="s">
         <v>669</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="I74" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="J74" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="K74" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="L74" s="2" t="s">
+      <c r="L74" s="4" t="s">
         <v>673</v>
       </c>
-      <c r="M74" s="2" t="s">
+      <c r="M74" s="4" t="s">
         <v>674</v>
       </c>
-      <c r="N74" s="2" t="s">
+      <c r="N74" s="4" t="s">
         <v>675</v>
       </c>
-      <c r="O74" s="2" t="s">
+      <c r="O74" s="4" t="s">
         <v>676</v>
       </c>
-      <c r="P74" s="2" t="s">
+      <c r="P74" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="Q74" s="2" t="s">
+      <c r="Q74" s="4" t="s">
         <v>678</v>
       </c>
     </row>
@@ -11804,52 +11804,52 @@
       <c r="A75" s="1">
         <v>1</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="4" t="s">
         <v>680</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" s="4" t="s">
         <v>681</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F75" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" s="4" t="s">
         <v>684</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H75" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="I75" s="4" t="s">
         <v>686</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="J75" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="K75" s="4" t="s">
         <v>688</v>
       </c>
-      <c r="L75" s="2" t="s">
+      <c r="L75" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="M75" s="2" t="s">
+      <c r="M75" s="4" t="s">
         <v>690</v>
       </c>
-      <c r="N75" s="2" t="s">
+      <c r="N75" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="O75" s="2" t="s">
+      <c r="O75" s="4" t="s">
         <v>692</v>
       </c>
-      <c r="P75" s="2" t="s">
+      <c r="P75" s="4" t="s">
         <v>693</v>
       </c>
-      <c r="Q75" s="2" t="s">
+      <c r="Q75" s="4" t="s">
         <v>694</v>
       </c>
     </row>
@@ -11857,52 +11857,52 @@
       <c r="A76" s="1">
         <v>2</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E76" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F76" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G76" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="H76" s="4" t="s">
         <v>701</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="I76" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="J76" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="K76" s="2" t="s">
+      <c r="K76" s="4" t="s">
         <v>704</v>
       </c>
-      <c r="L76" s="2" t="s">
+      <c r="L76" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="M76" s="2" t="s">
+      <c r="M76" s="4" t="s">
         <v>706</v>
       </c>
-      <c r="N76" s="2" t="s">
+      <c r="N76" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="O76" s="2" t="s">
+      <c r="O76" s="4" t="s">
         <v>708</v>
       </c>
-      <c r="P76" s="2" t="s">
+      <c r="P76" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="Q76" s="2" t="s">
+      <c r="Q76" s="4" t="s">
         <v>710</v>
       </c>
     </row>
@@ -11910,52 +11910,52 @@
       <c r="A77" s="1">
         <v>3</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D77" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E77" s="4" t="s">
         <v>714</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F77" s="4" t="s">
         <v>715</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G77" s="4" t="s">
         <v>716</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="H77" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="I77" s="4" t="s">
         <v>718</v>
       </c>
-      <c r="J77" s="2" t="s">
+      <c r="J77" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="K77" s="2" t="s">
+      <c r="K77" s="4" t="s">
         <v>720</v>
       </c>
-      <c r="L77" s="2" t="s">
+      <c r="L77" s="4" t="s">
         <v>721</v>
       </c>
-      <c r="M77" s="2" t="s">
+      <c r="M77" s="4" t="s">
         <v>722</v>
       </c>
-      <c r="N77" s="2" t="s">
+      <c r="N77" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="O77" s="2" t="s">
+      <c r="O77" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="P77" s="2" t="s">
+      <c r="P77" s="4" t="s">
         <v>725</v>
       </c>
-      <c r="Q77" s="2" t="s">
+      <c r="Q77" s="4" t="s">
         <v>726</v>
       </c>
     </row>
@@ -11963,52 +11963,52 @@
       <c r="A78" s="1">
         <v>4</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I78" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="J78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="K78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="L78" s="2" t="s">
+      <c r="L78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="M78" s="2" t="s">
+      <c r="M78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="N78" s="2" t="s">
+      <c r="N78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="O78" s="2" t="s">
+      <c r="O78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="P78" s="2" t="s">
+      <c r="P78" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="Q78" s="2" t="s">
+      <c r="Q78" s="4" t="s">
         <v>728</v>
       </c>
     </row>
@@ -12016,52 +12016,52 @@
       <c r="A79" s="1">
         <v>5</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="H79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I79" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="J79" s="2" t="s">
+      <c r="J79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="K79" s="2" t="s">
+      <c r="K79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="L79" s="2" t="s">
+      <c r="L79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="M79" s="2" t="s">
+      <c r="M79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="N79" s="2" t="s">
+      <c r="N79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="O79" s="2" t="s">
+      <c r="O79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="P79" s="2" t="s">
+      <c r="P79" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="Q79" s="2" t="s">
+      <c r="Q79" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -12069,52 +12069,52 @@
       <c r="A80" s="1">
         <v>6</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="G80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="H80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="I80" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="J80" s="2" t="s">
+      <c r="J80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="K80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="L80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="M80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="N80" s="2" t="s">
+      <c r="N80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="O80" s="2" t="s">
+      <c r="O80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="P80" s="2" t="s">
+      <c r="P80" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="Q80" s="2" t="s">
+      <c r="Q80" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -12122,52 +12122,52 @@
       <c r="A81" s="1">
         <v>7</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="G81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="H81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="I81" s="2" t="s">
+      <c r="I81" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="J81" s="2" t="s">
+      <c r="J81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="K81" s="2" t="s">
+      <c r="K81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="L81" s="2" t="s">
+      <c r="L81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="M81" s="2" t="s">
+      <c r="M81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="N81" s="2" t="s">
+      <c r="N81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="O81" s="2" t="s">
+      <c r="O81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="P81" s="2" t="s">
+      <c r="P81" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="Q81" s="2" t="s">
+      <c r="Q81" s="4" t="s">
         <v>734</v>
       </c>
     </row>
@@ -12175,52 +12175,52 @@
       <c r="A82" s="1">
         <v>8</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D82" s="4" t="s">
         <v>737</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="E82" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F82" s="4" t="s">
         <v>739</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="G82" s="4" t="s">
         <v>740</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H82" s="4" t="s">
         <v>741</v>
       </c>
-      <c r="I82" s="2" t="s">
+      <c r="I82" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="J82" s="4" t="s">
         <v>743</v>
       </c>
-      <c r="K82" s="2" t="s">
+      <c r="K82" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="L82" s="2" t="s">
+      <c r="L82" s="4" t="s">
         <v>745</v>
       </c>
-      <c r="M82" s="2" t="s">
+      <c r="M82" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="N82" s="2" t="s">
+      <c r="N82" s="4" t="s">
         <v>747</v>
       </c>
-      <c r="O82" s="2" t="s">
+      <c r="O82" s="4" t="s">
         <v>748</v>
       </c>
-      <c r="P82" s="2" t="s">
+      <c r="P82" s="4" t="s">
         <v>749</v>
       </c>
-      <c r="Q82" s="2" t="s">
+      <c r="Q82" s="4" t="s">
         <v>750</v>
       </c>
     </row>
@@ -12228,52 +12228,52 @@
       <c r="A83" s="1">
         <v>9</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="4" t="s">
         <v>751</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="4" t="s">
         <v>752</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D83" s="4" t="s">
         <v>753</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="E83" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F83" s="4" t="s">
         <v>755</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G83" s="4" t="s">
         <v>756</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="H83" s="4" t="s">
         <v>757</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="I83" s="4" t="s">
         <v>758</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="J83" s="4" t="s">
         <v>759</v>
       </c>
-      <c r="K83" s="2" t="s">
+      <c r="K83" s="4" t="s">
         <v>760</v>
       </c>
-      <c r="L83" s="2" t="s">
+      <c r="L83" s="4" t="s">
         <v>761</v>
       </c>
-      <c r="M83" s="2" t="s">
+      <c r="M83" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="N83" s="2" t="s">
+      <c r="N83" s="4" t="s">
         <v>763</v>
       </c>
-      <c r="O83" s="2" t="s">
+      <c r="O83" s="4" t="s">
         <v>764</v>
       </c>
-      <c r="P83" s="2" t="s">
+      <c r="P83" s="4" t="s">
         <v>765</v>
       </c>
-      <c r="Q83" s="2" t="s">
+      <c r="Q83" s="4" t="s">
         <v>766</v>
       </c>
     </row>
@@ -12281,52 +12281,52 @@
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="4" t="s">
         <v>767</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="4" t="s">
         <v>768</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D84" s="4" t="s">
         <v>769</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="E84" s="4" t="s">
         <v>770</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F84" s="4" t="s">
         <v>771</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="G84" s="4" t="s">
         <v>772</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="H84" s="4" t="s">
         <v>773</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I84" s="4" t="s">
         <v>774</v>
       </c>
-      <c r="J84" s="2" t="s">
+      <c r="J84" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="K84" s="2" t="s">
+      <c r="K84" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="L84" s="2" t="s">
+      <c r="L84" s="4" t="s">
         <v>777</v>
       </c>
-      <c r="M84" s="2" t="s">
+      <c r="M84" s="4" t="s">
         <v>778</v>
       </c>
-      <c r="N84" s="2" t="s">
+      <c r="N84" s="4" t="s">
         <v>779</v>
       </c>
-      <c r="O84" s="2" t="s">
+      <c r="O84" s="4" t="s">
         <v>780</v>
       </c>
-      <c r="P84" s="2" t="s">
+      <c r="P84" s="4" t="s">
         <v>781</v>
       </c>
-      <c r="Q84" s="2" t="s">
+      <c r="Q84" s="4" t="s">
         <v>782</v>
       </c>
     </row>
@@ -12334,52 +12334,52 @@
       <c r="A85" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="4" t="s">
         <v>783</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="4" t="s">
         <v>784</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D85" s="4" t="s">
         <v>785</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E85" s="4" t="s">
         <v>786</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F85" s="4" t="s">
         <v>787</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="G85" s="4" t="s">
         <v>788</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="H85" s="4" t="s">
         <v>789</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="I85" s="4" t="s">
         <v>790</v>
       </c>
-      <c r="J85" s="2" t="s">
+      <c r="J85" s="4" t="s">
         <v>791</v>
       </c>
-      <c r="K85" s="2" t="s">
+      <c r="K85" s="4" t="s">
         <v>792</v>
       </c>
-      <c r="L85" s="2" t="s">
+      <c r="L85" s="4" t="s">
         <v>793</v>
       </c>
-      <c r="M85" s="2" t="s">
+      <c r="M85" s="4" t="s">
         <v>794</v>
       </c>
-      <c r="N85" s="2" t="s">
+      <c r="N85" s="4" t="s">
         <v>795</v>
       </c>
-      <c r="O85" s="2" t="s">
+      <c r="O85" s="4" t="s">
         <v>796</v>
       </c>
-      <c r="P85" s="2" t="s">
+      <c r="P85" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="Q85" s="2" t="s">
+      <c r="Q85" s="4" t="s">
         <v>798</v>
       </c>
     </row>
@@ -12387,52 +12387,52 @@
       <c r="A86" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="4" t="s">
         <v>799</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="4" t="s">
         <v>800</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D86" s="4" t="s">
         <v>801</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E86" s="4" t="s">
         <v>802</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F86" s="4" t="s">
         <v>803</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="G86" s="4" t="s">
         <v>804</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="H86" s="4" t="s">
         <v>805</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="I86" s="4" t="s">
         <v>806</v>
       </c>
-      <c r="J86" s="2" t="s">
+      <c r="J86" s="4" t="s">
         <v>807</v>
       </c>
-      <c r="K86" s="2" t="s">
+      <c r="K86" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="L86" s="2" t="s">
+      <c r="L86" s="4" t="s">
         <v>809</v>
       </c>
-      <c r="M86" s="2" t="s">
+      <c r="M86" s="4" t="s">
         <v>810</v>
       </c>
-      <c r="N86" s="2" t="s">
+      <c r="N86" s="4" t="s">
         <v>811</v>
       </c>
-      <c r="O86" s="2" t="s">
+      <c r="O86" s="4" t="s">
         <v>812</v>
       </c>
-      <c r="P86" s="2" t="s">
+      <c r="P86" s="4" t="s">
         <v>813</v>
       </c>
-      <c r="Q86" s="2" t="s">
+      <c r="Q86" s="4" t="s">
         <v>814</v>
       </c>
     </row>
@@ -12440,52 +12440,52 @@
       <c r="A87" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="4" t="s">
         <v>815</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="4" t="s">
         <v>816</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="D87" s="4" t="s">
         <v>817</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="E87" s="4" t="s">
         <v>818</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F87" s="4" t="s">
         <v>819</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G87" s="4" t="s">
         <v>820</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="H87" s="4" t="s">
         <v>821</v>
       </c>
-      <c r="I87" s="2" t="s">
+      <c r="I87" s="4" t="s">
         <v>822</v>
       </c>
-      <c r="J87" s="2" t="s">
+      <c r="J87" s="4" t="s">
         <v>823</v>
       </c>
-      <c r="K87" s="2" t="s">
+      <c r="K87" s="4" t="s">
         <v>824</v>
       </c>
-      <c r="L87" s="2" t="s">
+      <c r="L87" s="4" t="s">
         <v>825</v>
       </c>
-      <c r="M87" s="2" t="s">
+      <c r="M87" s="4" t="s">
         <v>826</v>
       </c>
-      <c r="N87" s="2" t="s">
+      <c r="N87" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="O87" s="2" t="s">
+      <c r="O87" s="4" t="s">
         <v>828</v>
       </c>
-      <c r="P87" s="2" t="s">
+      <c r="P87" s="4" t="s">
         <v>829</v>
       </c>
-      <c r="Q87" s="2" t="s">
+      <c r="Q87" s="4" t="s">
         <v>830</v>
       </c>
     </row>
@@ -12493,52 +12493,52 @@
       <c r="A88" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="4" t="s">
         <v>831</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="4" t="s">
         <v>832</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D88" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E88" s="4" t="s">
         <v>834</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F88" s="4" t="s">
         <v>835</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="G88" s="4" t="s">
         <v>836</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="H88" s="4" t="s">
         <v>837</v>
       </c>
-      <c r="I88" s="2" t="s">
+      <c r="I88" s="4" t="s">
         <v>838</v>
       </c>
-      <c r="J88" s="2" t="s">
+      <c r="J88" s="4" t="s">
         <v>839</v>
       </c>
-      <c r="K88" s="2" t="s">
+      <c r="K88" s="4" t="s">
         <v>840</v>
       </c>
-      <c r="L88" s="2" t="s">
+      <c r="L88" s="4" t="s">
         <v>841</v>
       </c>
-      <c r="M88" s="2" t="s">
+      <c r="M88" s="4" t="s">
         <v>842</v>
       </c>
-      <c r="N88" s="2" t="s">
+      <c r="N88" s="4" t="s">
         <v>843</v>
       </c>
-      <c r="O88" s="2" t="s">
+      <c r="O88" s="4" t="s">
         <v>844</v>
       </c>
-      <c r="P88" s="2" t="s">
+      <c r="P88" s="4" t="s">
         <v>845</v>
       </c>
-      <c r="Q88" s="2" t="s">
+      <c r="Q88" s="4" t="s">
         <v>846</v>
       </c>
     </row>
@@ -12546,52 +12546,52 @@
       <c r="A89" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="4" t="s">
         <v>847</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="4" t="s">
         <v>848</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D89" s="4" t="s">
         <v>849</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E89" s="4" t="s">
         <v>850</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F89" s="4" t="s">
         <v>851</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="G89" s="4" t="s">
         <v>852</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="H89" s="4" t="s">
         <v>853</v>
       </c>
-      <c r="I89" s="2" t="s">
+      <c r="I89" s="4" t="s">
         <v>854</v>
       </c>
-      <c r="J89" s="2" t="s">
+      <c r="J89" s="4" t="s">
         <v>855</v>
       </c>
-      <c r="K89" s="2" t="s">
+      <c r="K89" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="L89" s="2" t="s">
+      <c r="L89" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="M89" s="2" t="s">
+      <c r="M89" s="4" t="s">
         <v>858</v>
       </c>
-      <c r="N89" s="2" t="s">
+      <c r="N89" s="4" t="s">
         <v>859</v>
       </c>
-      <c r="O89" s="2" t="s">
+      <c r="O89" s="4" t="s">
         <v>860</v>
       </c>
-      <c r="P89" s="2" t="s">
+      <c r="P89" s="4" t="s">
         <v>861</v>
       </c>
-      <c r="Q89" s="2" t="s">
+      <c r="Q89" s="4" t="s">
         <v>862</v>
       </c>
     </row>
@@ -13217,52 +13217,52 @@
       <c r="A114" s="1">
         <v>0</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="4" t="s">
         <v>950</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="4" t="s">
         <v>951</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D114" s="4" t="s">
         <v>952</v>
       </c>
-      <c r="E114" s="2" t="s">
+      <c r="E114" s="4" t="s">
         <v>953</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="F114" s="4" t="s">
         <v>954</v>
       </c>
-      <c r="G114" s="2" t="s">
+      <c r="G114" s="4" t="s">
         <v>955</v>
       </c>
-      <c r="H114" s="2" t="s">
+      <c r="H114" s="4" t="s">
         <v>956</v>
       </c>
-      <c r="I114" s="2" t="s">
+      <c r="I114" s="4" t="s">
         <v>957</v>
       </c>
-      <c r="J114" s="2" t="s">
+      <c r="J114" s="4" t="s">
         <v>958</v>
       </c>
-      <c r="K114" s="2" t="s">
+      <c r="K114" s="4" t="s">
         <v>959</v>
       </c>
-      <c r="L114" s="2" t="s">
+      <c r="L114" s="4" t="s">
         <v>960</v>
       </c>
-      <c r="M114" s="2" t="s">
+      <c r="M114" s="4" t="s">
         <v>961</v>
       </c>
-      <c r="N114" s="2" t="s">
+      <c r="N114" s="4" t="s">
         <v>962</v>
       </c>
-      <c r="O114" s="2" t="s">
+      <c r="O114" s="4" t="s">
         <v>963</v>
       </c>
-      <c r="P114" s="2" t="s">
+      <c r="P114" s="4" t="s">
         <v>964</v>
       </c>
-      <c r="Q114" s="2" t="s">
+      <c r="Q114" s="4" t="s">
         <v>965</v>
       </c>
     </row>
@@ -13270,52 +13270,52 @@
       <c r="A115" s="1">
         <v>1</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" s="4" t="s">
         <v>966</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="4" t="s">
         <v>967</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D115" s="4" t="s">
         <v>968</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="E115" s="4" t="s">
         <v>969</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="F115" s="4" t="s">
         <v>970</v>
       </c>
-      <c r="G115" s="2" t="s">
+      <c r="G115" s="4" t="s">
         <v>971</v>
       </c>
-      <c r="H115" s="2" t="s">
+      <c r="H115" s="4" t="s">
         <v>972</v>
       </c>
-      <c r="I115" s="2" t="s">
+      <c r="I115" s="4" t="s">
         <v>973</v>
       </c>
-      <c r="J115" s="2" t="s">
+      <c r="J115" s="4" t="s">
         <v>974</v>
       </c>
-      <c r="K115" s="2" t="s">
+      <c r="K115" s="4" t="s">
         <v>975</v>
       </c>
-      <c r="L115" s="2" t="s">
+      <c r="L115" s="4" t="s">
         <v>976</v>
       </c>
-      <c r="M115" s="2" t="s">
+      <c r="M115" s="4" t="s">
         <v>977</v>
       </c>
-      <c r="N115" s="2" t="s">
+      <c r="N115" s="4" t="s">
         <v>978</v>
       </c>
-      <c r="O115" s="2" t="s">
+      <c r="O115" s="4" t="s">
         <v>979</v>
       </c>
-      <c r="P115" s="2" t="s">
+      <c r="P115" s="4" t="s">
         <v>980</v>
       </c>
-      <c r="Q115" s="2" t="s">
+      <c r="Q115" s="4" t="s">
         <v>981</v>
       </c>
     </row>
@@ -13323,52 +13323,52 @@
       <c r="A116" s="1">
         <v>2</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="4" t="s">
         <v>982</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="4" t="s">
         <v>983</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="D116" s="4" t="s">
         <v>984</v>
       </c>
-      <c r="E116" s="2" t="s">
+      <c r="E116" s="4" t="s">
         <v>985</v>
       </c>
-      <c r="F116" s="2" t="s">
+      <c r="F116" s="4" t="s">
         <v>986</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="G116" s="4" t="s">
         <v>987</v>
       </c>
-      <c r="H116" s="2" t="s">
+      <c r="H116" s="4" t="s">
         <v>988</v>
       </c>
-      <c r="I116" s="2" t="s">
+      <c r="I116" s="4" t="s">
         <v>989</v>
       </c>
-      <c r="J116" s="2" t="s">
+      <c r="J116" s="4" t="s">
         <v>990</v>
       </c>
-      <c r="K116" s="2" t="s">
+      <c r="K116" s="4" t="s">
         <v>991</v>
       </c>
-      <c r="L116" s="2" t="s">
+      <c r="L116" s="4" t="s">
         <v>992</v>
       </c>
-      <c r="M116" s="2" t="s">
+      <c r="M116" s="4" t="s">
         <v>993</v>
       </c>
-      <c r="N116" s="2" t="s">
+      <c r="N116" s="4" t="s">
         <v>994</v>
       </c>
-      <c r="O116" s="2" t="s">
+      <c r="O116" s="4" t="s">
         <v>995</v>
       </c>
-      <c r="P116" s="2" t="s">
+      <c r="P116" s="4" t="s">
         <v>996</v>
       </c>
-      <c r="Q116" s="2" t="s">
+      <c r="Q116" s="4" t="s">
         <v>997</v>
       </c>
     </row>
@@ -13376,52 +13376,52 @@
       <c r="A117" s="1">
         <v>3</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="4" t="s">
         <v>998</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="4" t="s">
         <v>999</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="D117" s="4" t="s">
         <v>1000</v>
       </c>
-      <c r="E117" s="2" t="s">
+      <c r="E117" s="4" t="s">
         <v>1001</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="F117" s="4" t="s">
         <v>1002</v>
       </c>
-      <c r="G117" s="2" t="s">
+      <c r="G117" s="4" t="s">
         <v>1003</v>
       </c>
-      <c r="H117" s="2" t="s">
+      <c r="H117" s="4" t="s">
         <v>1004</v>
       </c>
-      <c r="I117" s="2" t="s">
+      <c r="I117" s="4" t="s">
         <v>1005</v>
       </c>
-      <c r="J117" s="2" t="s">
+      <c r="J117" s="4" t="s">
         <v>1006</v>
       </c>
-      <c r="K117" s="2" t="s">
+      <c r="K117" s="4" t="s">
         <v>1007</v>
       </c>
-      <c r="L117" s="2" t="s">
+      <c r="L117" s="4" t="s">
         <v>1008</v>
       </c>
-      <c r="M117" s="2" t="s">
+      <c r="M117" s="4" t="s">
         <v>1009</v>
       </c>
-      <c r="N117" s="2" t="s">
+      <c r="N117" s="4" t="s">
         <v>1010</v>
       </c>
-      <c r="O117" s="2" t="s">
+      <c r="O117" s="4" t="s">
         <v>1011</v>
       </c>
-      <c r="P117" s="2" t="s">
+      <c r="P117" s="4" t="s">
         <v>1012</v>
       </c>
-      <c r="Q117" s="2" t="s">
+      <c r="Q117" s="4" t="s">
         <v>1013</v>
       </c>
     </row>
@@ -13429,52 +13429,52 @@
       <c r="A118" s="1">
         <v>4</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="D118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="E118" s="2" t="s">
+      <c r="E118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="F118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="G118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="H118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="I118" s="2" t="s">
+      <c r="I118" s="4" t="s">
         <v>1014</v>
       </c>
-      <c r="J118" s="2" t="s">
+      <c r="J118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="K118" s="2" t="s">
+      <c r="K118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="L118" s="2" t="s">
+      <c r="L118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="M118" s="2" t="s">
+      <c r="M118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="N118" s="2" t="s">
+      <c r="N118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="O118" s="2" t="s">
+      <c r="O118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="P118" s="2" t="s">
+      <c r="P118" s="4" t="s">
         <v>1015</v>
       </c>
-      <c r="Q118" s="2" t="s">
+      <c r="Q118" s="4" t="s">
         <v>1015</v>
       </c>
     </row>
@@ -13482,52 +13482,52 @@
       <c r="A119" s="1">
         <v>5</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="D119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="E119" s="2" t="s">
+      <c r="E119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="F119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="G119" s="2" t="s">
+      <c r="G119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="H119" s="2" t="s">
+      <c r="H119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="I119" s="2" t="s">
+      <c r="I119" s="4" t="s">
         <v>1016</v>
       </c>
-      <c r="J119" s="2" t="s">
+      <c r="J119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="K119" s="2" t="s">
+      <c r="K119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="L119" s="2" t="s">
+      <c r="L119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="M119" s="2" t="s">
+      <c r="M119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="N119" s="2" t="s">
+      <c r="N119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="O119" s="2" t="s">
+      <c r="O119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="P119" s="2" t="s">
+      <c r="P119" s="4" t="s">
         <v>1017</v>
       </c>
-      <c r="Q119" s="2" t="s">
+      <c r="Q119" s="4" t="s">
         <v>1017</v>
       </c>
     </row>
@@ -13535,52 +13535,52 @@
       <c r="A120" s="1">
         <v>6</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="D120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="E120" s="2" t="s">
+      <c r="E120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="F120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="G120" s="2" t="s">
+      <c r="G120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="H120" s="2" t="s">
+      <c r="H120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="I120" s="2" t="s">
+      <c r="I120" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="J120" s="2" t="s">
+      <c r="J120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="K120" s="2" t="s">
+      <c r="K120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="L120" s="2" t="s">
+      <c r="L120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="M120" s="2" t="s">
+      <c r="M120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="N120" s="2" t="s">
+      <c r="N120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="O120" s="2" t="s">
+      <c r="O120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="P120" s="2" t="s">
+      <c r="P120" s="4" t="s">
         <v>1019</v>
       </c>
-      <c r="Q120" s="2" t="s">
+      <c r="Q120" s="4" t="s">
         <v>1019</v>
       </c>
     </row>
@@ -13588,52 +13588,52 @@
       <c r="A121" s="1">
         <v>7</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="E121" s="2" t="s">
+      <c r="E121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="F121" s="2" t="s">
+      <c r="F121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="G121" s="2" t="s">
+      <c r="G121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="H121" s="2" t="s">
+      <c r="H121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="I121" s="2" t="s">
+      <c r="I121" s="4" t="s">
         <v>1020</v>
       </c>
-      <c r="J121" s="2" t="s">
+      <c r="J121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="K121" s="2" t="s">
+      <c r="K121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="L121" s="2" t="s">
+      <c r="L121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="M121" s="2" t="s">
+      <c r="M121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="N121" s="2" t="s">
+      <c r="N121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="O121" s="2" t="s">
+      <c r="O121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="P121" s="2" t="s">
+      <c r="P121" s="4" t="s">
         <v>1021</v>
       </c>
-      <c r="Q121" s="2" t="s">
+      <c r="Q121" s="4" t="s">
         <v>1021</v>
       </c>
     </row>
@@ -13641,52 +13641,52 @@
       <c r="A122" s="1">
         <v>8</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="4" t="s">
         <v>1022</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="4" t="s">
         <v>1023</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D122" s="4" t="s">
         <v>1024</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="E122" s="4" t="s">
         <v>1025</v>
       </c>
-      <c r="F122" s="2" t="s">
+      <c r="F122" s="4" t="s">
         <v>1026</v>
       </c>
-      <c r="G122" s="2" t="s">
+      <c r="G122" s="4" t="s">
         <v>1027</v>
       </c>
-      <c r="H122" s="2" t="s">
+      <c r="H122" s="4" t="s">
         <v>1028</v>
       </c>
-      <c r="I122" s="2" t="s">
+      <c r="I122" s="4" t="s">
         <v>1029</v>
       </c>
-      <c r="J122" s="2" t="s">
+      <c r="J122" s="4" t="s">
         <v>1030</v>
       </c>
-      <c r="K122" s="2" t="s">
+      <c r="K122" s="4" t="s">
         <v>1031</v>
       </c>
-      <c r="L122" s="2" t="s">
+      <c r="L122" s="4" t="s">
         <v>1032</v>
       </c>
-      <c r="M122" s="2" t="s">
+      <c r="M122" s="4" t="s">
         <v>1033</v>
       </c>
-      <c r="N122" s="2" t="s">
+      <c r="N122" s="4" t="s">
         <v>1034</v>
       </c>
-      <c r="O122" s="2" t="s">
+      <c r="O122" s="4" t="s">
         <v>1035</v>
       </c>
-      <c r="P122" s="2" t="s">
+      <c r="P122" s="4" t="s">
         <v>1036</v>
       </c>
-      <c r="Q122" s="2" t="s">
+      <c r="Q122" s="4" t="s">
         <v>1037</v>
       </c>
     </row>
@@ -13694,52 +13694,52 @@
       <c r="A123" s="1">
         <v>9</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="4" t="s">
         <v>1038</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="4" t="s">
         <v>1039</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D123" s="4" t="s">
         <v>1040</v>
       </c>
-      <c r="E123" s="2" t="s">
+      <c r="E123" s="4" t="s">
         <v>1041</v>
       </c>
-      <c r="F123" s="2" t="s">
+      <c r="F123" s="4" t="s">
         <v>1042</v>
       </c>
-      <c r="G123" s="2" t="s">
+      <c r="G123" s="4" t="s">
         <v>1043</v>
       </c>
-      <c r="H123" s="2" t="s">
+      <c r="H123" s="4" t="s">
         <v>1044</v>
       </c>
-      <c r="I123" s="2" t="s">
+      <c r="I123" s="4" t="s">
         <v>1045</v>
       </c>
-      <c r="J123" s="2" t="s">
+      <c r="J123" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="K123" s="2" t="s">
+      <c r="K123" s="4" t="s">
         <v>1047</v>
       </c>
-      <c r="L123" s="2" t="s">
+      <c r="L123" s="4" t="s">
         <v>1048</v>
       </c>
-      <c r="M123" s="2" t="s">
+      <c r="M123" s="4" t="s">
         <v>1049</v>
       </c>
-      <c r="N123" s="2" t="s">
+      <c r="N123" s="4" t="s">
         <v>1050</v>
       </c>
-      <c r="O123" s="2" t="s">
+      <c r="O123" s="4" t="s">
         <v>1051</v>
       </c>
-      <c r="P123" s="2" t="s">
+      <c r="P123" s="4" t="s">
         <v>1052</v>
       </c>
-      <c r="Q123" s="2" t="s">
+      <c r="Q123" s="4" t="s">
         <v>1053</v>
       </c>
     </row>
@@ -13747,52 +13747,52 @@
       <c r="A124" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" s="4" t="s">
         <v>1054</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="4" t="s">
         <v>1055</v>
       </c>
-      <c r="D124" s="2" t="s">
+      <c r="D124" s="4" t="s">
         <v>1056</v>
       </c>
-      <c r="E124" s="2" t="s">
+      <c r="E124" s="4" t="s">
         <v>1057</v>
       </c>
-      <c r="F124" s="2" t="s">
+      <c r="F124" s="4" t="s">
         <v>1058</v>
       </c>
-      <c r="G124" s="2" t="s">
+      <c r="G124" s="4" t="s">
         <v>1059</v>
       </c>
-      <c r="H124" s="2" t="s">
+      <c r="H124" s="4" t="s">
         <v>1060</v>
       </c>
-      <c r="I124" s="2" t="s">
+      <c r="I124" s="4" t="s">
         <v>1061</v>
       </c>
-      <c r="J124" s="2" t="s">
+      <c r="J124" s="4" t="s">
         <v>1062</v>
       </c>
-      <c r="K124" s="2" t="s">
+      <c r="K124" s="4" t="s">
         <v>1063</v>
       </c>
-      <c r="L124" s="2" t="s">
+      <c r="L124" s="4" t="s">
         <v>1064</v>
       </c>
-      <c r="M124" s="2" t="s">
+      <c r="M124" s="4" t="s">
         <v>1065</v>
       </c>
-      <c r="N124" s="2" t="s">
+      <c r="N124" s="4" t="s">
         <v>1066</v>
       </c>
-      <c r="O124" s="2" t="s">
+      <c r="O124" s="4" t="s">
         <v>1067</v>
       </c>
-      <c r="P124" s="2" t="s">
+      <c r="P124" s="4" t="s">
         <v>1068</v>
       </c>
-      <c r="Q124" s="2" t="s">
+      <c r="Q124" s="4" t="s">
         <v>1069</v>
       </c>
     </row>
@@ -13800,52 +13800,52 @@
       <c r="A125" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B125" s="4" t="s">
         <v>1070</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="4" t="s">
         <v>1071</v>
       </c>
-      <c r="D125" s="2" t="s">
+      <c r="D125" s="4" t="s">
         <v>1072</v>
       </c>
-      <c r="E125" s="2" t="s">
+      <c r="E125" s="4" t="s">
         <v>1073</v>
       </c>
-      <c r="F125" s="2" t="s">
+      <c r="F125" s="4" t="s">
         <v>1074</v>
       </c>
-      <c r="G125" s="2" t="s">
+      <c r="G125" s="4" t="s">
         <v>1075</v>
       </c>
-      <c r="H125" s="2" t="s">
+      <c r="H125" s="4" t="s">
         <v>1076</v>
       </c>
-      <c r="I125" s="2" t="s">
+      <c r="I125" s="4" t="s">
         <v>1077</v>
       </c>
-      <c r="J125" s="2" t="s">
+      <c r="J125" s="4" t="s">
         <v>1078</v>
       </c>
-      <c r="K125" s="2" t="s">
+      <c r="K125" s="4" t="s">
         <v>1079</v>
       </c>
-      <c r="L125" s="2" t="s">
+      <c r="L125" s="4" t="s">
         <v>1080</v>
       </c>
-      <c r="M125" s="2" t="s">
+      <c r="M125" s="4" t="s">
         <v>1081</v>
       </c>
-      <c r="N125" s="2" t="s">
+      <c r="N125" s="4" t="s">
         <v>1082</v>
       </c>
-      <c r="O125" s="2" t="s">
+      <c r="O125" s="4" t="s">
         <v>1083</v>
       </c>
-      <c r="P125" s="2" t="s">
+      <c r="P125" s="4" t="s">
         <v>1084</v>
       </c>
-      <c r="Q125" s="2" t="s">
+      <c r="Q125" s="4" t="s">
         <v>1085</v>
       </c>
     </row>
@@ -13853,52 +13853,52 @@
       <c r="A126" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B126" s="4" t="s">
         <v>1086</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="4" t="s">
         <v>1087</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="D126" s="4" t="s">
         <v>1088</v>
       </c>
-      <c r="E126" s="2" t="s">
+      <c r="E126" s="4" t="s">
         <v>1089</v>
       </c>
-      <c r="F126" s="2" t="s">
+      <c r="F126" s="4" t="s">
         <v>1090</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="G126" s="4" t="s">
         <v>1091</v>
       </c>
-      <c r="H126" s="2" t="s">
+      <c r="H126" s="4" t="s">
         <v>1092</v>
       </c>
-      <c r="I126" s="2" t="s">
+      <c r="I126" s="4" t="s">
         <v>1093</v>
       </c>
-      <c r="J126" s="2" t="s">
+      <c r="J126" s="4" t="s">
         <v>1094</v>
       </c>
-      <c r="K126" s="2" t="s">
+      <c r="K126" s="4" t="s">
         <v>1095</v>
       </c>
-      <c r="L126" s="2" t="s">
+      <c r="L126" s="4" t="s">
         <v>1096</v>
       </c>
-      <c r="M126" s="2" t="s">
+      <c r="M126" s="4" t="s">
         <v>1097</v>
       </c>
-      <c r="N126" s="2" t="s">
+      <c r="N126" s="4" t="s">
         <v>1098</v>
       </c>
-      <c r="O126" s="2" t="s">
+      <c r="O126" s="4" t="s">
         <v>1099</v>
       </c>
-      <c r="P126" s="2" t="s">
+      <c r="P126" s="4" t="s">
         <v>1100</v>
       </c>
-      <c r="Q126" s="2" t="s">
+      <c r="Q126" s="4" t="s">
         <v>1101</v>
       </c>
     </row>
@@ -13906,52 +13906,52 @@
       <c r="A127" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="4" t="s">
         <v>1102</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="4" t="s">
         <v>1103</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D127" s="4" t="s">
         <v>1104</v>
       </c>
-      <c r="E127" s="2" t="s">
+      <c r="E127" s="4" t="s">
         <v>1105</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="F127" s="4" t="s">
         <v>1106</v>
       </c>
-      <c r="G127" s="2" t="s">
+      <c r="G127" s="4" t="s">
         <v>1107</v>
       </c>
-      <c r="H127" s="2" t="s">
+      <c r="H127" s="4" t="s">
         <v>1108</v>
       </c>
-      <c r="I127" s="2" t="s">
+      <c r="I127" s="4" t="s">
         <v>1109</v>
       </c>
-      <c r="J127" s="2" t="s">
+      <c r="J127" s="4" t="s">
         <v>1110</v>
       </c>
-      <c r="K127" s="2" t="s">
+      <c r="K127" s="4" t="s">
         <v>1111</v>
       </c>
-      <c r="L127" s="2" t="s">
+      <c r="L127" s="4" t="s">
         <v>1112</v>
       </c>
-      <c r="M127" s="2" t="s">
+      <c r="M127" s="4" t="s">
         <v>1113</v>
       </c>
-      <c r="N127" s="2" t="s">
+      <c r="N127" s="4" t="s">
         <v>1114</v>
       </c>
-      <c r="O127" s="2" t="s">
+      <c r="O127" s="4" t="s">
         <v>1115</v>
       </c>
-      <c r="P127" s="2" t="s">
+      <c r="P127" s="4" t="s">
         <v>1116</v>
       </c>
-      <c r="Q127" s="2" t="s">
+      <c r="Q127" s="4" t="s">
         <v>1117</v>
       </c>
     </row>
@@ -13959,52 +13959,52 @@
       <c r="A128" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="4" t="s">
         <v>1118</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="4" t="s">
         <v>1119</v>
       </c>
-      <c r="D128" s="2" t="s">
+      <c r="D128" s="4" t="s">
         <v>1120</v>
       </c>
-      <c r="E128" s="2" t="s">
+      <c r="E128" s="4" t="s">
         <v>1121</v>
       </c>
-      <c r="F128" s="2" t="s">
+      <c r="F128" s="4" t="s">
         <v>1122</v>
       </c>
-      <c r="G128" s="2" t="s">
+      <c r="G128" s="4" t="s">
         <v>1123</v>
       </c>
-      <c r="H128" s="2" t="s">
+      <c r="H128" s="4" t="s">
         <v>1124</v>
       </c>
-      <c r="I128" s="2" t="s">
+      <c r="I128" s="4" t="s">
         <v>1125</v>
       </c>
-      <c r="J128" s="2" t="s">
+      <c r="J128" s="4" t="s">
         <v>1126</v>
       </c>
-      <c r="K128" s="2" t="s">
+      <c r="K128" s="4" t="s">
         <v>1127</v>
       </c>
-      <c r="L128" s="2" t="s">
+      <c r="L128" s="4" t="s">
         <v>1128</v>
       </c>
-      <c r="M128" s="2" t="s">
+      <c r="M128" s="4" t="s">
         <v>1129</v>
       </c>
-      <c r="N128" s="2" t="s">
+      <c r="N128" s="4" t="s">
         <v>1130</v>
       </c>
-      <c r="O128" s="2" t="s">
+      <c r="O128" s="4" t="s">
         <v>1131</v>
       </c>
-      <c r="P128" s="2" t="s">
+      <c r="P128" s="4" t="s">
         <v>1132</v>
       </c>
-      <c r="Q128" s="2" t="s">
+      <c r="Q128" s="4" t="s">
         <v>1133</v>
       </c>
     </row>
@@ -14012,52 +14012,52 @@
       <c r="A129" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" s="4" t="s">
         <v>1134</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="4" t="s">
         <v>1135</v>
       </c>
-      <c r="D129" s="2" t="s">
+      <c r="D129" s="4" t="s">
         <v>1136</v>
       </c>
-      <c r="E129" s="2" t="s">
+      <c r="E129" s="4" t="s">
         <v>1137</v>
       </c>
-      <c r="F129" s="2" t="s">
+      <c r="F129" s="4" t="s">
         <v>1138</v>
       </c>
-      <c r="G129" s="2" t="s">
+      <c r="G129" s="4" t="s">
         <v>1139</v>
       </c>
-      <c r="H129" s="2" t="s">
+      <c r="H129" s="4" t="s">
         <v>1140</v>
       </c>
-      <c r="I129" s="2" t="s">
+      <c r="I129" s="4" t="s">
         <v>1141</v>
       </c>
-      <c r="J129" s="2" t="s">
+      <c r="J129" s="4" t="s">
         <v>1142</v>
       </c>
-      <c r="K129" s="2" t="s">
+      <c r="K129" s="4" t="s">
         <v>1143</v>
       </c>
-      <c r="L129" s="2" t="s">
+      <c r="L129" s="4" t="s">
         <v>1144</v>
       </c>
-      <c r="M129" s="2" t="s">
+      <c r="M129" s="4" t="s">
         <v>1145</v>
       </c>
-      <c r="N129" s="2" t="s">
+      <c r="N129" s="4" t="s">
         <v>1146</v>
       </c>
-      <c r="O129" s="2" t="s">
+      <c r="O129" s="4" t="s">
         <v>1147</v>
       </c>
-      <c r="P129" s="2" t="s">
+      <c r="P129" s="4" t="s">
         <v>1148</v>
       </c>
-      <c r="Q129" s="2" t="s">
+      <c r="Q129" s="4" t="s">
         <v>1149</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Parser refactored. Now all unit tests run.
</commit_message>
<xml_diff>
--- a/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
+++ b/AntlrZ80Asm/AntlrZ80Asm.Test/OperationTestState.xlsx
@@ -8979,8 +8979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9054,10 +9054,10 @@
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -9069,7 +9069,7 @@
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -9081,7 +9081,7 @@
       <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -9093,7 +9093,7 @@
       <c r="O4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Q4" s="4" t="s">
@@ -9107,10 +9107,10 @@
       <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -9122,7 +9122,7 @@
       <c r="G5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -9134,7 +9134,7 @@
       <c r="K5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="M5" s="4" t="s">
@@ -9146,7 +9146,7 @@
       <c r="O5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="4" t="s">
         <v>36</v>
       </c>
       <c r="Q5" s="4" t="s">
@@ -9160,10 +9160,10 @@
       <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -9175,7 +9175,7 @@
       <c r="G6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -9187,7 +9187,7 @@
       <c r="K6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="4" t="s">
         <v>48</v>
       </c>
       <c r="M6" s="4" t="s">
@@ -9199,7 +9199,7 @@
       <c r="O6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="4" t="s">
         <v>52</v>
       </c>
       <c r="Q6" s="4" t="s">
@@ -9213,10 +9213,10 @@
       <c r="B7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -9228,7 +9228,7 @@
       <c r="G7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="4" t="s">
         <v>60</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -9240,7 +9240,7 @@
       <c r="K7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="4" t="s">
         <v>64</v>
       </c>
       <c r="M7" s="4" t="s">
@@ -9252,7 +9252,7 @@
       <c r="O7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="4" t="s">
         <v>68</v>
       </c>
       <c r="Q7" s="4" t="s">
@@ -9263,52 +9263,52 @@
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="N8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="4" t="s">
         <v>85</v>
       </c>
     </row>
@@ -9316,52 +9316,52 @@
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="N9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q9" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -9369,52 +9369,52 @@
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="N10" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -9422,52 +9422,52 @@
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="N11" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P11" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="4" t="s">
         <v>133</v>
       </c>
     </row>
@@ -9867,7 +9867,7 @@
       <c r="J19" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="4" t="s">
         <v>252</v>
       </c>
       <c r="L19" s="4" t="s">
@@ -9956,7 +9956,7 @@
       <c r="D24" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="4" t="s">
         <v>263</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -9968,7 +9968,7 @@
       <c r="H24" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="4" t="s">
         <v>267</v>
       </c>
       <c r="J24" s="4" t="s">
@@ -9980,7 +9980,7 @@
       <c r="L24" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="M24" s="4" t="s">
         <v>271</v>
       </c>
       <c r="N24" s="4" t="s">
@@ -9992,7 +9992,7 @@
       <c r="P24" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="Q24" s="4" t="s">
         <v>274</v>
       </c>
     </row>
@@ -10009,7 +10009,7 @@
       <c r="D25" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="4" t="s">
         <v>278</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -10021,7 +10021,7 @@
       <c r="H25" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="4" t="s">
         <v>280</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -10033,7 +10033,7 @@
       <c r="L25" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="M25" s="4" t="s">
         <v>284</v>
       </c>
       <c r="N25" s="4" t="s">
@@ -10045,7 +10045,7 @@
       <c r="P25" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="Q25" s="2" t="s">
+      <c r="Q25" s="4" t="s">
         <v>286</v>
       </c>
     </row>
@@ -10062,7 +10062,7 @@
       <c r="D26" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -10086,7 +10086,7 @@
       <c r="L26" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="M26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="N26" s="4" t="s">
@@ -10115,7 +10115,7 @@
       <c r="D27" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="4" t="s">
         <v>298</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -10137,7 +10137,7 @@
       <c r="L27" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="4" t="s">
         <v>302</v>
       </c>
       <c r="N27" s="4" t="s">
@@ -11236,10 +11236,10 @@
         <v>2</v>
       </c>
       <c r="B56" s="2"/>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="4" t="s">
         <v>580</v>
       </c>
       <c r="E56" s="4" t="s">
@@ -11251,7 +11251,7 @@
       <c r="G56" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="4" t="s">
         <v>584</v>
       </c>
       <c r="I56" s="2"/>
@@ -11259,7 +11259,7 @@
       <c r="K56" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="L56" s="2" t="s">
+      <c r="L56" s="4" t="s">
         <v>586</v>
       </c>
       <c r="M56" s="4" t="s">
@@ -11271,7 +11271,7 @@
       <c r="O56" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="P56" s="2" t="s">
+      <c r="P56" s="4" t="s">
         <v>590</v>
       </c>
       <c r="Q56" s="2"/>
@@ -11290,7 +11290,7 @@
       <c r="G57" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="4" t="s">
         <v>593</v>
       </c>
       <c r="I57" s="2"/>
@@ -11313,13 +11313,13 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="H58" s="4" t="s">
         <v>597</v>
       </c>
       <c r="I58" s="2"/>
@@ -11327,13 +11327,13 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
-      <c r="N58" s="2" t="s">
+      <c r="N58" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="O58" s="2" t="s">
+      <c r="O58" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="P58" s="2" t="s">
+      <c r="P58" s="4" t="s">
         <v>600</v>
       </c>
       <c r="Q58" s="2"/>
@@ -11346,13 +11346,13 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="4" t="s">
         <v>603</v>
       </c>
       <c r="I59" s="2"/>
@@ -11360,13 +11360,13 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
-      <c r="N59" s="2" t="s">
+      <c r="N59" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="O59" s="2" t="s">
+      <c r="O59" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="P59" s="2" t="s">
+      <c r="P59" s="4" t="s">
         <v>606</v>
       </c>
       <c r="Q59" s="2"/>
@@ -11375,52 +11375,52 @@
       <c r="A60" s="1">
         <v>6</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="4" t="s">
         <v>608</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H60" s="4" t="s">
         <v>613</v>
       </c>
-      <c r="I60" s="2" t="s">
+      <c r="I60" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="J60" s="2" t="s">
+      <c r="J60" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="K60" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="L60" s="2" t="s">
+      <c r="L60" s="4" t="s">
         <v>617</v>
       </c>
-      <c r="M60" s="2" t="s">
+      <c r="M60" s="4" t="s">
         <v>618</v>
       </c>
-      <c r="N60" s="2" t="s">
+      <c r="N60" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="O60" s="2" t="s">
+      <c r="O60" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="P60" s="2" t="s">
+      <c r="P60" s="4" t="s">
         <v>621</v>
       </c>
-      <c r="Q60" s="2" t="s">
+      <c r="Q60" s="4" t="s">
         <v>622</v>
       </c>
     </row>
@@ -11428,39 +11428,39 @@
       <c r="A61" s="1">
         <v>7</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="4" t="s">
         <v>626</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F61" s="4" t="s">
         <v>627</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G61" s="4" t="s">
         <v>628</v>
       </c>
       <c r="H61" s="2"/>
-      <c r="I61" s="2" t="s">
+      <c r="I61" s="4" t="s">
         <v>629</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
-      <c r="N61" s="2" t="s">
+      <c r="N61" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="O61" s="2" t="s">
+      <c r="O61" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="P61" s="2" t="s">
+      <c r="P61" s="4" t="s">
         <v>632</v>
       </c>
       <c r="Q61" s="2"/>
@@ -11681,7 +11681,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
-      <c r="K69" s="2" t="s">
+      <c r="K69" s="4" t="s">
         <v>661</v>
       </c>
       <c r="L69" s="2"/>
@@ -12702,10 +12702,10 @@
         <v>2</v>
       </c>
       <c r="B96" s="2"/>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="4" t="s">
         <v>866</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D96" s="4" t="s">
         <v>867</v>
       </c>
       <c r="E96" s="4" t="s">
@@ -12717,7 +12717,7 @@
       <c r="G96" s="4" t="s">
         <v>870</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="H96" s="4" t="s">
         <v>871</v>
       </c>
       <c r="I96" s="2"/>
@@ -12725,7 +12725,7 @@
       <c r="K96" s="4" t="s">
         <v>872</v>
       </c>
-      <c r="L96" s="2" t="s">
+      <c r="L96" s="4" t="s">
         <v>873</v>
       </c>
       <c r="M96" s="4" t="s">
@@ -12737,7 +12737,7 @@
       <c r="O96" s="4" t="s">
         <v>876</v>
       </c>
-      <c r="P96" s="2" t="s">
+      <c r="P96" s="4" t="s">
         <v>877</v>
       </c>
       <c r="Q96" s="2"/>
@@ -12756,7 +12756,7 @@
       <c r="G97" s="4" t="s">
         <v>879</v>
       </c>
-      <c r="H97" s="2" t="s">
+      <c r="H97" s="4" t="s">
         <v>880</v>
       </c>
       <c r="I97" s="2"/>
@@ -12779,13 +12779,13 @@
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
-      <c r="F98" s="2" t="s">
+      <c r="F98" s="4" t="s">
         <v>882</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="G98" s="4" t="s">
         <v>883</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="H98" s="4" t="s">
         <v>884</v>
       </c>
       <c r="I98" s="2"/>
@@ -12793,13 +12793,13 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
-      <c r="N98" s="2" t="s">
+      <c r="N98" s="4" t="s">
         <v>885</v>
       </c>
-      <c r="O98" s="2" t="s">
+      <c r="O98" s="4" t="s">
         <v>886</v>
       </c>
-      <c r="P98" s="2" t="s">
+      <c r="P98" s="4" t="s">
         <v>887</v>
       </c>
       <c r="Q98" s="2"/>
@@ -12812,13 +12812,13 @@
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
-      <c r="F99" s="2" t="s">
+      <c r="F99" s="4" t="s">
         <v>888</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="G99" s="4" t="s">
         <v>889</v>
       </c>
-      <c r="H99" s="2" t="s">
+      <c r="H99" s="4" t="s">
         <v>890</v>
       </c>
       <c r="I99" s="2"/>
@@ -12826,13 +12826,13 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
-      <c r="N99" s="2" t="s">
+      <c r="N99" s="4" t="s">
         <v>891</v>
       </c>
-      <c r="O99" s="2" t="s">
+      <c r="O99" s="4" t="s">
         <v>892</v>
       </c>
-      <c r="P99" s="2" t="s">
+      <c r="P99" s="4" t="s">
         <v>893</v>
       </c>
       <c r="Q99" s="2"/>
@@ -12841,52 +12841,52 @@
       <c r="A100" s="1">
         <v>6</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="4" t="s">
         <v>894</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="4" t="s">
         <v>895</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D100" s="4" t="s">
         <v>896</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="E100" s="4" t="s">
         <v>897</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F100" s="4" t="s">
         <v>898</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="G100" s="4" t="s">
         <v>899</v>
       </c>
-      <c r="H100" s="2" t="s">
+      <c r="H100" s="4" t="s">
         <v>900</v>
       </c>
-      <c r="I100" s="2" t="s">
+      <c r="I100" s="4" t="s">
         <v>901</v>
       </c>
-      <c r="J100" s="2" t="s">
+      <c r="J100" s="4" t="s">
         <v>902</v>
       </c>
-      <c r="K100" s="2" t="s">
+      <c r="K100" s="4" t="s">
         <v>903</v>
       </c>
-      <c r="L100" s="2" t="s">
+      <c r="L100" s="4" t="s">
         <v>904</v>
       </c>
-      <c r="M100" s="2" t="s">
+      <c r="M100" s="4" t="s">
         <v>905</v>
       </c>
-      <c r="N100" s="2" t="s">
+      <c r="N100" s="4" t="s">
         <v>906</v>
       </c>
-      <c r="O100" s="2" t="s">
+      <c r="O100" s="4" t="s">
         <v>907</v>
       </c>
-      <c r="P100" s="2" t="s">
+      <c r="P100" s="4" t="s">
         <v>908</v>
       </c>
-      <c r="Q100" s="2" t="s">
+      <c r="Q100" s="4" t="s">
         <v>909</v>
       </c>
     </row>
@@ -12894,39 +12894,39 @@
       <c r="A101" s="1">
         <v>7</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="4" t="s">
         <v>910</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="4" t="s">
         <v>911</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D101" s="4" t="s">
         <v>912</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E101" s="4" t="s">
         <v>913</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F101" s="4" t="s">
         <v>914</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="G101" s="4" t="s">
         <v>915</v>
       </c>
       <c r="H101" s="2"/>
-      <c r="I101" s="2" t="s">
+      <c r="I101" s="4" t="s">
         <v>916</v>
       </c>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
-      <c r="N101" s="2" t="s">
+      <c r="N101" s="4" t="s">
         <v>917</v>
       </c>
-      <c r="O101" s="2" t="s">
+      <c r="O101" s="4" t="s">
         <v>918</v>
       </c>
-      <c r="P101" s="2" t="s">
+      <c r="P101" s="4" t="s">
         <v>919</v>
       </c>
       <c r="Q101" s="2"/>
@@ -12939,13 +12939,13 @@
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
-      <c r="F102" s="2" t="s">
+      <c r="F102" s="4" t="s">
         <v>920</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="G102" s="4" t="s">
         <v>921</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="H102" s="4" t="s">
         <v>922</v>
       </c>
       <c r="I102" s="2"/>
@@ -12953,13 +12953,13 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
-      <c r="N102" s="2" t="s">
+      <c r="N102" s="4" t="s">
         <v>923</v>
       </c>
-      <c r="O102" s="2" t="s">
+      <c r="O102" s="4" t="s">
         <v>924</v>
       </c>
-      <c r="P102" s="2" t="s">
+      <c r="P102" s="4" t="s">
         <v>925</v>
       </c>
       <c r="Q102" s="2"/>
@@ -12972,13 +12972,13 @@
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
-      <c r="F103" s="2" t="s">
+      <c r="F103" s="4" t="s">
         <v>926</v>
       </c>
-      <c r="G103" s="2" t="s">
+      <c r="G103" s="4" t="s">
         <v>927</v>
       </c>
-      <c r="H103" s="2" t="s">
+      <c r="H103" s="4" t="s">
         <v>928</v>
       </c>
       <c r="I103" s="2"/>
@@ -12986,13 +12986,13 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
-      <c r="N103" s="2" t="s">
+      <c r="N103" s="4" t="s">
         <v>929</v>
       </c>
-      <c r="O103" s="2" t="s">
+      <c r="O103" s="4" t="s">
         <v>930</v>
       </c>
-      <c r="P103" s="2" t="s">
+      <c r="P103" s="4" t="s">
         <v>931</v>
       </c>
       <c r="Q103" s="2"/>
@@ -13005,13 +13005,13 @@
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
-      <c r="F104" s="2" t="s">
+      <c r="F104" s="4" t="s">
         <v>932</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="G104" s="4" t="s">
         <v>933</v>
       </c>
-      <c r="H104" s="2" t="s">
+      <c r="H104" s="4" t="s">
         <v>934</v>
       </c>
       <c r="I104" s="2"/>
@@ -13019,13 +13019,13 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
-      <c r="N104" s="2" t="s">
+      <c r="N104" s="4" t="s">
         <v>935</v>
       </c>
-      <c r="O104" s="2" t="s">
+      <c r="O104" s="4" t="s">
         <v>936</v>
       </c>
-      <c r="P104" s="2" t="s">
+      <c r="P104" s="4" t="s">
         <v>937</v>
       </c>
       <c r="Q104" s="2"/>
@@ -13038,13 +13038,13 @@
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
-      <c r="F105" s="2" t="s">
+      <c r="F105" s="4" t="s">
         <v>938</v>
       </c>
-      <c r="G105" s="2" t="s">
+      <c r="G105" s="4" t="s">
         <v>939</v>
       </c>
-      <c r="H105" s="2" t="s">
+      <c r="H105" s="4" t="s">
         <v>940</v>
       </c>
       <c r="I105" s="2"/>
@@ -13052,13 +13052,13 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
-      <c r="N105" s="2" t="s">
+      <c r="N105" s="4" t="s">
         <v>941</v>
       </c>
-      <c r="O105" s="2" t="s">
+      <c r="O105" s="4" t="s">
         <v>942</v>
       </c>
-      <c r="P105" s="2" t="s">
+      <c r="P105" s="4" t="s">
         <v>943</v>
       </c>
       <c r="Q105" s="2"/>
@@ -13147,7 +13147,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
-      <c r="K109" s="2" t="s">
+      <c r="K109" s="4" t="s">
         <v>948</v>
       </c>
       <c r="L109" s="2"/>

</xml_diff>